<commit_message>
updating spreadsheet to use purchased AMY file
Also made copy of logan DDY to use with this.
</commit_message>
<xml_diff>
--- a/projects/office_calibration_nsga2_14.xlsx
+++ b/projects/office_calibration_nsga2_14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -2179,9 +2179,6 @@
     <t>ChangeBuildingLocation</t>
   </si>
   <si>
-    <t>USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
-  </si>
-  <si>
     <t>weather_file_name</t>
   </si>
   <si>
@@ -2477,6 +2474,9 @@
   </si>
   <si>
     <t>2013-12-12</t>
+  </si>
+  <si>
+    <t>SPtMasterTable_15084_2013_amy.epw</t>
   </si>
 </sst>
 </file>
@@ -6738,17 +6738,17 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="81.6640625" customWidth="1"/>
+    <col min="1" max="1" width="81.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.8">
+    <row r="1" spans="1:1" ht="45">
       <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="28.8">
+    <row r="2" spans="1:1" ht="30">
       <c r="A2" s="36" t="s">
         <v>41</v>
       </c>
@@ -6772,14 +6772,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.6640625" style="1"/>
+    <col min="4" max="4" width="33.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6811,7 +6811,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1" t="s">
         <v>456</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72">
+    <row r="5" spans="1:5" ht="75">
       <c r="A5" s="1" t="s">
         <v>469</v>
       </c>
@@ -6833,18 +6833,18 @@
         <v>614</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="46.2" customHeight="1">
+    <row r="6" spans="1:5" ht="46.15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1" t="s">
         <v>442</v>
       </c>
@@ -6863,7 +6863,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="1" t="s">
         <v>443</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>471</v>
@@ -6920,10 +6920,10 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6931,10 +6931,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6948,7 +6948,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="1" t="s">
         <v>463</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="57.6">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A20" s="11" t="s">
         <v>27</v>
       </c>
@@ -7006,7 +7006,7 @@
       <c r="B22" s="26"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="57.6">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A23" s="11" t="s">
         <v>450</v>
       </c>
@@ -7119,13 +7119,13 @@
     </row>
     <row r="32" spans="1:5" s="31" customFormat="1">
       <c r="A32" s="31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B32" s="30">
         <v>1</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D32" s="35"/>
     </row>
@@ -7144,12 +7144,12 @@
       <c r="C35" s="26"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="43.2">
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="45">
       <c r="A36" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>31</v>
@@ -7165,7 +7165,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8">
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="30">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>38</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>449</v>
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E40" s="2"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="57.6">
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="60">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="13" t="s">
@@ -7217,7 +7217,7 @@
         <v>699</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1">
@@ -7251,36 +7251,36 @@
   <dimension ref="A1:Y224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD108"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="31" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="31" customWidth="1"/>
     <col min="2" max="2" width="47" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="31" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="31" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
-    <col min="13" max="14" width="7.6640625" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" style="31"/>
-    <col min="16" max="16" width="11.44140625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="31" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="31" customWidth="1"/>
+    <col min="13" max="14" width="7.7109375" style="31" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="31"/>
+    <col min="16" max="16" width="11.42578125" style="31" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
-    <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
-    <col min="19" max="19" width="46.109375" style="31" customWidth="1"/>
-    <col min="20" max="22" width="11.44140625" style="31"/>
-    <col min="23" max="23" width="13.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="11.44140625" style="31"/>
+    <col min="18" max="18" width="27.7109375" style="31" customWidth="1"/>
+    <col min="19" max="19" width="46.140625" style="31" customWidth="1"/>
+    <col min="20" max="22" width="11.42578125" style="31"/>
+    <col min="23" max="23" width="13.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18">
+    <row r="1" spans="1:25" ht="18.75">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -7315,7 +7315,7 @@
       <c r="X1" s="53"/>
       <c r="Y1" s="53"/>
     </row>
-    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.6">
+    <row r="2" spans="1:25" s="8" customFormat="1" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -7331,7 +7331,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:25" s="14" customFormat="1" ht="62.4">
+    <row r="3" spans="1:25" s="14" customFormat="1" ht="63">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -7429,16 +7429,16 @@
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>747</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>748</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>749</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="30" customFormat="1">
@@ -7446,16 +7446,16 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>104</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>712</v>
+        <v>811</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="38" customFormat="1">
@@ -7491,7 +7491,7 @@
         <v>618</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -7516,7 +7516,7 @@
         <v>618</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -7584,13 +7584,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>68</v>
@@ -7598,7 +7598,7 @@
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
     </row>
-    <row r="14" spans="1:25" ht="17.399999999999999">
+    <row r="14" spans="1:25" ht="18">
       <c r="A14" s="30"/>
       <c r="B14" s="30" t="s">
         <v>21</v>
@@ -7614,7 +7614,7 @@
         <v>64</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H14" s="52">
         <v>104666</v>
@@ -7654,7 +7654,7 @@
         <v>0.25</v>
       </c>
       <c r="Q15" s="51" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="30" customFormat="1">
@@ -7688,7 +7688,7 @@
         <v>64</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H17" s="43">
         <v>12</v>
@@ -7710,7 +7710,7 @@
         <v>0.5</v>
       </c>
       <c r="Q17" s="51" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1">
@@ -7718,10 +7718,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="30" t="s">
+        <v>717</v>
+      </c>
+      <c r="E18" s="30" t="s">
         <v>718</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>719</v>
       </c>
       <c r="F18" s="30" t="s">
         <v>64</v>
@@ -7735,10 +7735,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="30" t="s">
+        <v>719</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>720</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>721</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>64</v>
@@ -7752,10 +7752,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="30" t="s">
+        <v>721</v>
+      </c>
+      <c r="E20" s="30" t="s">
         <v>722</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>723</v>
       </c>
       <c r="F20" s="30" t="s">
         <v>64</v>
@@ -7769,10 +7769,10 @@
         <v>21</v>
       </c>
       <c r="D21" s="30" t="s">
+        <v>723</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>724</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>725</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>64</v>
@@ -7786,10 +7786,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="30" t="s">
+        <v>725</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>726</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>727</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>64</v>
@@ -7803,10 +7803,10 @@
         <v>21</v>
       </c>
       <c r="D23" s="30" t="s">
+        <v>727</v>
+      </c>
+      <c r="E23" s="30" t="s">
         <v>728</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>729</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>64</v>
@@ -7820,10 +7820,10 @@
         <v>21</v>
       </c>
       <c r="D24" s="30" t="s">
+        <v>729</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>730</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>731</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>64</v>
@@ -7837,10 +7837,10 @@
         <v>21</v>
       </c>
       <c r="D25" s="30" t="s">
+        <v>731</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>732</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>733</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>64</v>
@@ -7854,10 +7854,10 @@
         <v>21</v>
       </c>
       <c r="D26" s="30" t="s">
+        <v>733</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>734</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>735</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>64</v>
@@ -7871,10 +7871,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="30" t="s">
+        <v>735</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>736</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>737</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>64</v>
@@ -7888,10 +7888,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="30" t="s">
+        <v>737</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>738</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>739</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>64</v>
@@ -7905,10 +7905,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="30" t="s">
+        <v>739</v>
+      </c>
+      <c r="E29" s="30" t="s">
         <v>740</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>741</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>64</v>
@@ -7922,10 +7922,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="30" t="s">
+        <v>741</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>742</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>743</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>64</v>
@@ -7974,13 +7974,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="38" t="s">
+        <v>772</v>
+      </c>
+      <c r="C33" s="38" t="s">
         <v>773</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>774</v>
-      </c>
       <c r="D33" s="38" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E33" s="38" t="s">
         <v>68</v>
@@ -7993,10 +7993,10 @@
         <v>22</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>761</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>762</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>763</v>
       </c>
       <c r="F34" s="43" t="s">
         <v>64</v>
@@ -8021,7 +8021,7 @@
         <v>0.05</v>
       </c>
       <c r="Q34" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="35" spans="1:17" s="43" customFormat="1">
@@ -8029,10 +8029,10 @@
         <v>22</v>
       </c>
       <c r="D35" s="43" t="s">
+        <v>763</v>
+      </c>
+      <c r="E35" s="43" t="s">
         <v>764</v>
-      </c>
-      <c r="E35" s="43" t="s">
-        <v>765</v>
       </c>
       <c r="F35" s="43" t="s">
         <v>64</v>
@@ -8057,7 +8057,7 @@
         <v>0.05</v>
       </c>
       <c r="Q35" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="36" spans="1:17" s="38" customFormat="1">
@@ -8065,7 +8065,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>74</v>
@@ -8084,7 +8084,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E37" s="43" t="s">
         <v>75</v>
@@ -8093,7 +8093,7 @@
         <v>619</v>
       </c>
       <c r="G37" s="43" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H37" s="43">
         <v>0</v>
@@ -8115,7 +8115,7 @@
         <v>5</v>
       </c>
       <c r="Q37" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="38" customFormat="1">
@@ -8172,7 +8172,7 @@
       </c>
       <c r="P39" s="40"/>
       <c r="Q39" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -8279,7 +8279,7 @@
       </c>
       <c r="P43" s="40"/>
       <c r="Q43" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -8386,7 +8386,7 @@
       </c>
       <c r="P47" s="40"/>
       <c r="Q47" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -8493,7 +8493,7 @@
       </c>
       <c r="P51" s="40"/>
       <c r="Q51" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -8615,7 +8615,7 @@
         <v>618</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I57" s="31"/>
     </row>
@@ -8633,7 +8633,7 @@
         <v>618</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I58" s="31"/>
     </row>
@@ -8661,7 +8661,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C60" s="49" t="s">
         <v>76</v>
@@ -8678,7 +8678,7 @@
         <v>22</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E61" s="43" t="s">
         <v>77</v>
@@ -8706,7 +8706,7 @@
         <v>0.1</v>
       </c>
       <c r="Q61" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="30" customFormat="1">
@@ -8751,7 +8751,7 @@
         <v>1</v>
       </c>
       <c r="B64" s="49" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C64" s="49" t="s">
         <v>76</v>
@@ -8768,7 +8768,7 @@
         <v>22</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E65" s="43" t="s">
         <v>77</v>
@@ -8796,7 +8796,7 @@
         <v>0.1</v>
       </c>
       <c r="Q65" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="30" customFormat="1">
@@ -8841,7 +8841,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="49" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C68" s="49" t="s">
         <v>76</v>
@@ -8858,7 +8858,7 @@
         <v>22</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E69" s="43" t="s">
         <v>77</v>
@@ -8886,7 +8886,7 @@
         <v>0.1</v>
       </c>
       <c r="Q69" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="30" customFormat="1">
@@ -8969,7 +8969,7 @@
         <v>22</v>
       </c>
       <c r="D74" s="44" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E74" s="43" t="s">
         <v>70</v>
@@ -8997,7 +8997,7 @@
         <v>2.5</v>
       </c>
       <c r="Q74" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="30" customFormat="1">
@@ -9105,7 +9105,7 @@
         <v>22</v>
       </c>
       <c r="D80" s="43" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E80" s="43" t="s">
         <v>46</v>
@@ -9371,7 +9371,7 @@
         <v>22</v>
       </c>
       <c r="D90" s="43" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E90" s="43" t="s">
         <v>330</v>
@@ -9400,7 +9400,7 @@
         <v>2.5</v>
       </c>
       <c r="Q90" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="91" spans="1:17" s="50" customFormat="1">
@@ -9408,13 +9408,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="50" t="s">
+        <v>778</v>
+      </c>
+      <c r="C91" s="50" t="s">
         <v>779</v>
       </c>
-      <c r="C91" s="50" t="s">
-        <v>780</v>
-      </c>
       <c r="D91" s="50" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E91" s="50" t="s">
         <v>68</v>
@@ -9425,7 +9425,7 @@
         <v>22</v>
       </c>
       <c r="D92" s="43" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E92" s="43" t="s">
         <v>258</v>
@@ -9454,7 +9454,7 @@
         <v>2.5</v>
       </c>
       <c r="Q92" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="93" spans="1:17" s="50" customFormat="1">
@@ -9462,13 +9462,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="50" t="s">
+        <v>781</v>
+      </c>
+      <c r="C93" s="50" t="s">
         <v>782</v>
       </c>
-      <c r="C93" s="50" t="s">
-        <v>783</v>
-      </c>
       <c r="D93" s="50" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E93" s="50" t="s">
         <v>68</v>
@@ -9479,7 +9479,7 @@
         <v>22</v>
       </c>
       <c r="D94" s="43" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E94" s="43" t="s">
         <v>258</v>
@@ -9508,7 +9508,7 @@
         <v>2.5</v>
       </c>
       <c r="Q94" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="95" spans="1:17" s="50" customFormat="1">
@@ -9553,7 +9553,7 @@
         <v>22</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E97" s="43" t="s">
         <v>288</v>
@@ -9562,7 +9562,7 @@
         <v>64</v>
       </c>
       <c r="G97" s="43" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H97" s="43">
         <v>0</v>
@@ -9585,7 +9585,7 @@
         <v>2.5</v>
       </c>
       <c r="Q97" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="98" spans="1:17" s="30" customFormat="1">
@@ -9593,7 +9593,7 @@
         <v>21</v>
       </c>
       <c r="D98" s="30" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E98" s="30" t="s">
         <v>48</v>
@@ -9602,7 +9602,7 @@
         <v>64</v>
       </c>
       <c r="G98" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H98" s="30">
         <v>0</v>
@@ -9613,7 +9613,7 @@
         <v>21</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E99" s="30" t="s">
         <v>50</v>
@@ -9622,7 +9622,7 @@
         <v>64</v>
       </c>
       <c r="G99" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H99" s="30">
         <v>0</v>
@@ -9633,7 +9633,7 @@
         <v>21</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>52</v>
@@ -9642,7 +9642,7 @@
         <v>65</v>
       </c>
       <c r="G100" s="30" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H100" s="30">
         <v>0</v>
@@ -9653,7 +9653,7 @@
         <v>21</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E101" s="30" t="s">
         <v>54</v>
@@ -9670,7 +9670,7 @@
         <v>21</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E102" s="30" t="s">
         <v>56</v>
@@ -9679,7 +9679,7 @@
         <v>65</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H102" s="30">
         <v>15</v>
@@ -9690,7 +9690,7 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E103" s="30" t="s">
         <v>58</v>
@@ -9699,7 +9699,7 @@
         <v>64</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H103" s="30">
         <v>0</v>
@@ -9710,7 +9710,7 @@
         <v>21</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E104" s="30" t="s">
         <v>60</v>
@@ -9719,7 +9719,7 @@
         <v>65</v>
       </c>
       <c r="G104" s="30" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H104" s="30">
         <v>1</v>
@@ -9733,10 +9733,10 @@
         <v>187</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D105" s="38" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E105" s="38" t="s">
         <v>68</v>
@@ -9749,7 +9749,7 @@
         <v>22</v>
       </c>
       <c r="D106" s="43" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E106" s="43" t="s">
         <v>190</v>
@@ -9758,7 +9758,7 @@
         <v>64</v>
       </c>
       <c r="G106" s="43" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H106" s="43">
         <v>1</v>
@@ -9781,7 +9781,7 @@
         <v>1</v>
       </c>
       <c r="Q106" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="43" customFormat="1">
@@ -9789,7 +9789,7 @@
         <v>22</v>
       </c>
       <c r="D107" s="43" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E107" s="43" t="s">
         <v>192</v>
@@ -9798,7 +9798,7 @@
         <v>64</v>
       </c>
       <c r="G107" s="43" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="H107" s="43">
         <v>-1</v>
@@ -9821,7 +9821,7 @@
         <v>1</v>
       </c>
       <c r="Q107" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -9829,7 +9829,7 @@
         <v>21</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E108" s="31" t="s">
         <v>194</v>
@@ -10334,20 +10334,20 @@
       <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="29.44140625" style="31" customWidth="1"/>
+    <col min="1" max="2" width="29.42578125" style="31" customWidth="1"/>
     <col min="3" max="3" width="71" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.44140625" style="31" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="31" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" style="31" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="31"/>
+    <col min="4" max="4" width="10.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" style="31" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="31" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="31" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="31" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18">
+    <row r="1" spans="1:12" ht="18.75">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -10362,7 +10362,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.6">
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="15.75">
       <c r="A2" s="8" t="s">
         <v>459</v>
       </c>
@@ -10397,7 +10397,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" ht="46.8">
+    <row r="3" spans="1:12" s="14" customFormat="1" ht="47.25">
       <c r="A3" s="14" t="s">
         <v>628</v>
       </c>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>707</v>
@@ -10584,7 +10584,7 @@
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>709</v>
@@ -10608,14 +10608,14 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="30" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="30" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E10" s="31" t="s">
         <v>64</v>
@@ -10635,14 +10635,14 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="30" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>64</v>
@@ -10662,14 +10662,14 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="30" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E12" s="31" t="s">
         <v>64</v>
@@ -10689,14 +10689,14 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="30" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>64</v>
@@ -10757,19 +10757,19 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="17" t="b">
         <v>0</v>
       </c>
@@ -10788,7 +10788,7 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6">
+    <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>21</v>
@@ -10809,7 +10809,7 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="17"/>
       <c r="B3" s="17" t="s">
         <v>21</v>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="I3" s="17"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>21</v>
@@ -10855,7 +10855,7 @@
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="17"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:9" ht="15.6">
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="17"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
@@ -10901,7 +10901,7 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6">
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
@@ -10924,7 +10924,7 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6">
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
@@ -10947,7 +10947,7 @@
       </c>
       <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="15.6">
+    <row r="9" spans="1:9" ht="15.75">
       <c r="A9" s="17"/>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -10970,7 +10970,7 @@
       </c>
       <c r="I9" s="17"/>
     </row>
-    <row r="10" spans="1:9" ht="15.6">
+    <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="17"/>
       <c r="B10" s="17" t="s">
         <v>21</v>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="I10" s="17"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6">
+    <row r="11" spans="1:9" ht="15.75">
       <c r="A11" s="17" t="b">
         <v>0</v>
       </c>
@@ -11012,7 +11012,7 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6">
+    <row r="12" spans="1:9" ht="15.75">
       <c r="A12" s="17"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
@@ -11033,7 +11033,7 @@
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6">
+    <row r="13" spans="1:9" ht="15.75">
       <c r="A13" s="17"/>
       <c r="B13" s="17" t="s">
         <v>21</v>
@@ -11056,7 +11056,7 @@
       </c>
       <c r="I13" s="17"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6">
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="17"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
@@ -11079,7 +11079,7 @@
       </c>
       <c r="I14" s="17"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6">
+    <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="17"/>
       <c r="B15" s="17" t="s">
         <v>21</v>
@@ -11102,7 +11102,7 @@
       </c>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6">
+    <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>21</v>
@@ -11125,7 +11125,7 @@
       </c>
       <c r="I16" s="17"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6">
+    <row r="17" spans="1:9" ht="15.75">
       <c r="A17" s="17"/>
       <c r="B17" s="17" t="s">
         <v>21</v>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="I17" s="17"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6">
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>21</v>
@@ -11171,7 +11171,7 @@
       </c>
       <c r="I18" s="17"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6">
+    <row r="19" spans="1:9" ht="15.75">
       <c r="A19" s="17"/>
       <c r="B19" s="17" t="s">
         <v>21</v>
@@ -11194,7 +11194,7 @@
       </c>
       <c r="I19" s="17"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6">
+    <row r="20" spans="1:9" ht="15.75">
       <c r="A20" s="17"/>
       <c r="B20" s="17" t="s">
         <v>21</v>
@@ -11217,7 +11217,7 @@
       </c>
       <c r="I20" s="17"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6">
+    <row r="21" spans="1:9" ht="15.75">
       <c r="A21" s="17" t="b">
         <v>0</v>
       </c>
@@ -11236,7 +11236,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6">
+    <row r="22" spans="1:9" ht="15.75">
       <c r="A22" s="17"/>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -11259,7 +11259,7 @@
       </c>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6">
+    <row r="23" spans="1:9" ht="15.75">
       <c r="A23" s="17"/>
       <c r="B23" s="17" t="s">
         <v>21</v>
@@ -11282,7 +11282,7 @@
       </c>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6">
+    <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="17"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
@@ -11305,7 +11305,7 @@
       </c>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6">
+    <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="17"/>
       <c r="B25" s="17" t="s">
         <v>21</v>
@@ -11328,7 +11328,7 @@
       </c>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6">
+    <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="17"/>
       <c r="B26" s="17" t="s">
         <v>21</v>
@@ -11351,7 +11351,7 @@
       </c>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6">
+    <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="17"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
@@ -11374,7 +11374,7 @@
       </c>
       <c r="I27" s="17"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6">
+    <row r="28" spans="1:9" ht="15.75">
       <c r="A28" s="17"/>
       <c r="B28" s="17" t="s">
         <v>21</v>
@@ -11397,7 +11397,7 @@
       </c>
       <c r="I28" s="17"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6">
+    <row r="29" spans="1:9" ht="15.75">
       <c r="A29" s="17"/>
       <c r="B29" s="17" t="s">
         <v>21</v>
@@ -11420,7 +11420,7 @@
       </c>
       <c r="I29" s="17"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6">
+    <row r="30" spans="1:9" ht="15.75">
       <c r="A30" s="17"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="I30" s="17"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6">
+    <row r="31" spans="1:9" ht="15.75">
       <c r="A31" s="17" t="b">
         <v>0</v>
       </c>
@@ -11462,7 +11462,7 @@
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6">
+    <row r="32" spans="1:9" ht="15.75">
       <c r="A32" s="17"/>
       <c r="B32" s="17" t="s">
         <v>21</v>
@@ -11483,7 +11483,7 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6">
+    <row r="33" spans="1:9" ht="15.75">
       <c r="A33" s="17"/>
       <c r="B33" s="17" t="s">
         <v>21</v>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="I33" s="17"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6">
+    <row r="34" spans="1:9" ht="15.75">
       <c r="A34" s="17"/>
       <c r="B34" s="17" t="s">
         <v>21</v>
@@ -11529,7 +11529,7 @@
       </c>
       <c r="I34" s="17"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6">
+    <row r="35" spans="1:9" ht="15.75">
       <c r="A35" s="17"/>
       <c r="B35" s="17" t="s">
         <v>21</v>
@@ -11552,7 +11552,7 @@
       </c>
       <c r="I35" s="17"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6">
+    <row r="36" spans="1:9" ht="15.75">
       <c r="A36" s="17"/>
       <c r="B36" s="17" t="s">
         <v>21</v>
@@ -11575,7 +11575,7 @@
       </c>
       <c r="I36" s="17"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6">
+    <row r="37" spans="1:9" ht="15.75">
       <c r="A37" s="17"/>
       <c r="B37" s="17" t="s">
         <v>21</v>
@@ -11598,7 +11598,7 @@
       </c>
       <c r="I37" s="17"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6">
+    <row r="38" spans="1:9" ht="15.75">
       <c r="A38" s="17"/>
       <c r="B38" s="17" t="s">
         <v>21</v>
@@ -11621,7 +11621,7 @@
       </c>
       <c r="I38" s="17"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6">
+    <row r="39" spans="1:9" ht="15.75">
       <c r="A39" s="17"/>
       <c r="B39" s="17" t="s">
         <v>21</v>
@@ -11644,7 +11644,7 @@
       </c>
       <c r="I39" s="17"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6">
+    <row r="40" spans="1:9" ht="15.75">
       <c r="A40" s="17"/>
       <c r="B40" s="17" t="s">
         <v>21</v>
@@ -11667,7 +11667,7 @@
       </c>
       <c r="I40" s="17"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6">
+    <row r="41" spans="1:9" ht="15.75">
       <c r="A41" s="17" t="b">
         <v>0</v>
       </c>
@@ -11686,7 +11686,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6">
+    <row r="42" spans="1:9" ht="15.75">
       <c r="A42" s="17"/>
       <c r="B42" s="17" t="s">
         <v>21</v>
@@ -11707,7 +11707,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6">
+    <row r="43" spans="1:9" ht="15.75">
       <c r="A43" s="17"/>
       <c r="B43" s="17" t="s">
         <v>21</v>
@@ -11730,7 +11730,7 @@
       </c>
       <c r="I43" s="17"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6">
+    <row r="44" spans="1:9" ht="15.75">
       <c r="A44" s="17"/>
       <c r="B44" s="17" t="s">
         <v>21</v>
@@ -11753,7 +11753,7 @@
       </c>
       <c r="I44" s="17"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6">
+    <row r="45" spans="1:9" ht="15.75">
       <c r="A45" s="17"/>
       <c r="B45" s="17" t="s">
         <v>21</v>
@@ -11776,7 +11776,7 @@
       </c>
       <c r="I45" s="17"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6">
+    <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="17"/>
       <c r="B46" s="17" t="s">
         <v>21</v>
@@ -11799,7 +11799,7 @@
       </c>
       <c r="I46" s="17"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6">
+    <row r="47" spans="1:9" ht="15.75">
       <c r="A47" s="17"/>
       <c r="B47" s="17" t="s">
         <v>21</v>
@@ -11822,7 +11822,7 @@
       </c>
       <c r="I47" s="17"/>
     </row>
-    <row r="48" spans="1:9" ht="15.6">
+    <row r="48" spans="1:9" ht="15.75">
       <c r="A48" s="17"/>
       <c r="B48" s="17" t="s">
         <v>21</v>
@@ -11845,7 +11845,7 @@
       </c>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" ht="15.6">
+    <row r="49" spans="1:9" ht="15.75">
       <c r="A49" s="17"/>
       <c r="B49" s="17" t="s">
         <v>21</v>
@@ -11868,7 +11868,7 @@
       </c>
       <c r="I49" s="17"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6">
+    <row r="50" spans="1:9" ht="15.75">
       <c r="A50" s="17"/>
       <c r="B50" s="17" t="s">
         <v>21</v>
@@ -11891,7 +11891,7 @@
       </c>
       <c r="I50" s="17"/>
     </row>
-    <row r="51" spans="1:9" ht="15.6">
+    <row r="51" spans="1:9" ht="15.75">
       <c r="A51" s="17" t="b">
         <v>0</v>
       </c>
@@ -11910,7 +11910,7 @@
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
     </row>
-    <row r="52" spans="1:9" ht="15.6">
+    <row r="52" spans="1:9" ht="15.75">
       <c r="A52" s="17"/>
       <c r="B52" s="17" t="s">
         <v>21</v>
@@ -11931,7 +11931,7 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6">
+    <row r="53" spans="1:9" ht="15.75">
       <c r="A53" s="17"/>
       <c r="B53" s="17" t="s">
         <v>21</v>
@@ -11954,7 +11954,7 @@
       </c>
       <c r="I53" s="17"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6">
+    <row r="54" spans="1:9" ht="15.75">
       <c r="A54" s="17"/>
       <c r="B54" s="17" t="s">
         <v>21</v>
@@ -11977,7 +11977,7 @@
       </c>
       <c r="I54" s="17"/>
     </row>
-    <row r="55" spans="1:9" ht="15.6">
+    <row r="55" spans="1:9" ht="15.75">
       <c r="A55" s="17"/>
       <c r="B55" s="17" t="s">
         <v>21</v>
@@ -12000,7 +12000,7 @@
       </c>
       <c r="I55" s="17"/>
     </row>
-    <row r="56" spans="1:9" ht="15.6">
+    <row r="56" spans="1:9" ht="15.75">
       <c r="A56" s="17"/>
       <c r="B56" s="17" t="s">
         <v>21</v>
@@ -12023,7 +12023,7 @@
       </c>
       <c r="I56" s="17"/>
     </row>
-    <row r="57" spans="1:9" ht="15.6">
+    <row r="57" spans="1:9" ht="15.75">
       <c r="A57" s="17"/>
       <c r="B57" s="17" t="s">
         <v>21</v>
@@ -12046,7 +12046,7 @@
       </c>
       <c r="I57" s="17"/>
     </row>
-    <row r="58" spans="1:9" ht="15.6">
+    <row r="58" spans="1:9" ht="15.75">
       <c r="A58" s="17"/>
       <c r="B58" s="17" t="s">
         <v>21</v>
@@ -12069,7 +12069,7 @@
       </c>
       <c r="I58" s="17"/>
     </row>
-    <row r="59" spans="1:9" ht="15.6">
+    <row r="59" spans="1:9" ht="15.75">
       <c r="A59" s="17"/>
       <c r="B59" s="17" t="s">
         <v>21</v>
@@ -12092,7 +12092,7 @@
       </c>
       <c r="I59" s="17"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6">
+    <row r="60" spans="1:9" ht="15.75">
       <c r="A60" s="17"/>
       <c r="B60" s="17" t="s">
         <v>21</v>
@@ -12115,7 +12115,7 @@
       </c>
       <c r="I60" s="17"/>
     </row>
-    <row r="61" spans="1:9" ht="15.6">
+    <row r="61" spans="1:9" ht="15.75">
       <c r="A61" s="17" t="b">
         <v>0</v>
       </c>
@@ -12134,7 +12134,7 @@
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
     </row>
-    <row r="62" spans="1:9" ht="15.6">
+    <row r="62" spans="1:9" ht="15.75">
       <c r="A62" s="17"/>
       <c r="B62" s="17" t="s">
         <v>21</v>
@@ -12155,7 +12155,7 @@
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
     </row>
-    <row r="63" spans="1:9" ht="15.6">
+    <row r="63" spans="1:9" ht="15.75">
       <c r="A63" s="17"/>
       <c r="B63" s="17" t="s">
         <v>21</v>
@@ -12180,7 +12180,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6">
+    <row r="64" spans="1:9" ht="15.75">
       <c r="A64" s="17"/>
       <c r="B64" s="17" t="s">
         <v>21</v>
@@ -12203,7 +12203,7 @@
       </c>
       <c r="I64" s="17"/>
     </row>
-    <row r="65" spans="1:9" ht="15.6">
+    <row r="65" spans="1:9" ht="15.75">
       <c r="A65" s="17"/>
       <c r="B65" s="17" t="s">
         <v>21</v>
@@ -12226,7 +12226,7 @@
       </c>
       <c r="I65" s="17"/>
     </row>
-    <row r="66" spans="1:9" ht="15.6">
+    <row r="66" spans="1:9" ht="15.75">
       <c r="A66" s="17"/>
       <c r="B66" s="17" t="s">
         <v>21</v>
@@ -12249,7 +12249,7 @@
       </c>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="1:9" ht="15.6">
+    <row r="67" spans="1:9" ht="15.75">
       <c r="A67" s="17"/>
       <c r="B67" s="17" t="s">
         <v>21</v>
@@ -12272,7 +12272,7 @@
       </c>
       <c r="I67" s="17"/>
     </row>
-    <row r="68" spans="1:9" ht="15.6">
+    <row r="68" spans="1:9" ht="15.75">
       <c r="A68" s="17"/>
       <c r="B68" s="17" t="s">
         <v>21</v>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="I68" s="17"/>
     </row>
-    <row r="69" spans="1:9" ht="15.6">
+    <row r="69" spans="1:9" ht="15.75">
       <c r="A69" s="17"/>
       <c r="B69" s="17" t="s">
         <v>21</v>
@@ -12318,7 +12318,7 @@
       </c>
       <c r="I69" s="17"/>
     </row>
-    <row r="70" spans="1:9" ht="15.6">
+    <row r="70" spans="1:9" ht="15.75">
       <c r="A70" s="17"/>
       <c r="B70" s="17" t="s">
         <v>21</v>
@@ -12341,7 +12341,7 @@
       </c>
       <c r="I70" s="17"/>
     </row>
-    <row r="71" spans="1:9" ht="15.6">
+    <row r="71" spans="1:9" ht="15.75">
       <c r="A71" s="17"/>
       <c r="B71" s="17" t="s">
         <v>21</v>
@@ -12364,7 +12364,7 @@
       </c>
       <c r="I71" s="17"/>
     </row>
-    <row r="72" spans="1:9" ht="15.6">
+    <row r="72" spans="1:9" ht="15.75">
       <c r="A72" s="17" t="b">
         <v>0</v>
       </c>
@@ -12383,7 +12383,7 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
     </row>
-    <row r="73" spans="1:9" ht="15.6">
+    <row r="73" spans="1:9" ht="15.75">
       <c r="A73" s="17"/>
       <c r="B73" s="17" t="s">
         <v>21</v>
@@ -12404,7 +12404,7 @@
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
     </row>
-    <row r="74" spans="1:9" ht="15.6">
+    <row r="74" spans="1:9" ht="15.75">
       <c r="A74" s="17"/>
       <c r="B74" s="17" t="s">
         <v>21</v>
@@ -12427,7 +12427,7 @@
       </c>
       <c r="I74" s="17"/>
     </row>
-    <row r="75" spans="1:9" ht="15.6">
+    <row r="75" spans="1:9" ht="15.75">
       <c r="A75" s="17"/>
       <c r="B75" s="17" t="s">
         <v>21</v>
@@ -12452,7 +12452,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6">
+    <row r="76" spans="1:9" ht="15.75">
       <c r="A76" s="17"/>
       <c r="B76" s="17" t="s">
         <v>21</v>
@@ -12475,7 +12475,7 @@
       </c>
       <c r="I76" s="17"/>
     </row>
-    <row r="77" spans="1:9" ht="15.6">
+    <row r="77" spans="1:9" ht="15.75">
       <c r="A77" s="17"/>
       <c r="B77" s="17" t="s">
         <v>21</v>
@@ -12498,7 +12498,7 @@
       </c>
       <c r="I77" s="17"/>
     </row>
-    <row r="78" spans="1:9" ht="15.6">
+    <row r="78" spans="1:9" ht="15.75">
       <c r="A78" s="17"/>
       <c r="B78" s="17" t="s">
         <v>21</v>
@@ -12521,7 +12521,7 @@
       </c>
       <c r="I78" s="17"/>
     </row>
-    <row r="79" spans="1:9" ht="15.6">
+    <row r="79" spans="1:9" ht="15.75">
       <c r="A79" s="17"/>
       <c r="B79" s="17" t="s">
         <v>21</v>
@@ -12544,7 +12544,7 @@
       </c>
       <c r="I79" s="17"/>
     </row>
-    <row r="80" spans="1:9" ht="15.6">
+    <row r="80" spans="1:9" ht="15.75">
       <c r="A80" s="17"/>
       <c r="B80" s="17" t="s">
         <v>21</v>
@@ -12567,7 +12567,7 @@
       </c>
       <c r="I80" s="17"/>
     </row>
-    <row r="81" spans="1:9" ht="15.6">
+    <row r="81" spans="1:9" ht="15.75">
       <c r="A81" s="17"/>
       <c r="B81" s="17" t="s">
         <v>21</v>
@@ -12590,7 +12590,7 @@
       </c>
       <c r="I81" s="17"/>
     </row>
-    <row r="82" spans="1:9" ht="15.6">
+    <row r="82" spans="1:9" ht="15.75">
       <c r="A82" s="17"/>
       <c r="B82" s="17" t="s">
         <v>21</v>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="I82" s="17"/>
     </row>
-    <row r="83" spans="1:9" ht="15.6">
+    <row r="83" spans="1:9" ht="15.75">
       <c r="A83" s="17"/>
       <c r="B83" s="17" t="s">
         <v>21</v>
@@ -12636,7 +12636,7 @@
       </c>
       <c r="I83" s="17"/>
     </row>
-    <row r="84" spans="1:9" ht="15.6">
+    <row r="84" spans="1:9" ht="15.75">
       <c r="A84" s="17"/>
       <c r="B84" s="17" t="s">
         <v>21</v>
@@ -12659,7 +12659,7 @@
       </c>
       <c r="I84" s="17"/>
     </row>
-    <row r="85" spans="1:9" ht="15.6">
+    <row r="85" spans="1:9" ht="15.75">
       <c r="A85" s="17"/>
       <c r="B85" s="17" t="s">
         <v>21</v>
@@ -12682,7 +12682,7 @@
       </c>
       <c r="I85" s="17"/>
     </row>
-    <row r="86" spans="1:9" ht="15.6">
+    <row r="86" spans="1:9" ht="15.75">
       <c r="A86" s="17" t="b">
         <v>0</v>
       </c>
@@ -12701,7 +12701,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
     </row>
-    <row r="87" spans="1:9" ht="15.6">
+    <row r="87" spans="1:9" ht="15.75">
       <c r="A87" s="17"/>
       <c r="B87" s="17" t="s">
         <v>21</v>
@@ -12724,7 +12724,7 @@
       </c>
       <c r="I87" s="17"/>
     </row>
-    <row r="88" spans="1:9" ht="15.6">
+    <row r="88" spans="1:9" ht="15.75">
       <c r="A88" s="17"/>
       <c r="B88" s="17" t="s">
         <v>21</v>
@@ -12747,7 +12747,7 @@
       </c>
       <c r="I88" s="17"/>
     </row>
-    <row r="89" spans="1:9" ht="15.6">
+    <row r="89" spans="1:9" ht="15.75">
       <c r="A89" s="17"/>
       <c r="B89" s="17" t="s">
         <v>21</v>
@@ -12770,7 +12770,7 @@
       </c>
       <c r="I89" s="17"/>
     </row>
-    <row r="90" spans="1:9" ht="15.6">
+    <row r="90" spans="1:9" ht="15.75">
       <c r="A90" s="17"/>
       <c r="B90" s="17" t="s">
         <v>21</v>
@@ -12793,7 +12793,7 @@
       </c>
       <c r="I90" s="17"/>
     </row>
-    <row r="91" spans="1:9" ht="15.6">
+    <row r="91" spans="1:9" ht="15.75">
       <c r="A91" s="17"/>
       <c r="B91" s="17" t="s">
         <v>21</v>
@@ -12816,7 +12816,7 @@
       </c>
       <c r="I91" s="17"/>
     </row>
-    <row r="92" spans="1:9" ht="15.6">
+    <row r="92" spans="1:9" ht="15.75">
       <c r="A92" s="17"/>
       <c r="B92" s="17" t="s">
         <v>21</v>
@@ -12839,7 +12839,7 @@
       </c>
       <c r="I92" s="17"/>
     </row>
-    <row r="93" spans="1:9" ht="15.6">
+    <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="17"/>
       <c r="B93" s="17" t="s">
         <v>21</v>
@@ -12862,7 +12862,7 @@
       </c>
       <c r="I93" s="17"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6">
+    <row r="94" spans="1:9" ht="15.75">
       <c r="A94" s="17"/>
       <c r="B94" s="17" t="s">
         <v>21</v>
@@ -12885,7 +12885,7 @@
       </c>
       <c r="I94" s="17"/>
     </row>
-    <row r="95" spans="1:9" ht="15.6">
+    <row r="95" spans="1:9" ht="15.75">
       <c r="A95" s="17"/>
       <c r="B95" s="17" t="s">
         <v>21</v>
@@ -12908,7 +12908,7 @@
       </c>
       <c r="I95" s="17"/>
     </row>
-    <row r="96" spans="1:9" ht="15.6">
+    <row r="96" spans="1:9" ht="15.75">
       <c r="A96" s="17"/>
       <c r="B96" s="17" t="s">
         <v>21</v>
@@ -12931,7 +12931,7 @@
       </c>
       <c r="I96" s="17"/>
     </row>
-    <row r="97" spans="1:9" ht="15.6">
+    <row r="97" spans="1:9" ht="15.75">
       <c r="A97" s="17" t="b">
         <v>0</v>
       </c>
@@ -12950,7 +12950,7 @@
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
     </row>
-    <row r="98" spans="1:9" ht="15.6">
+    <row r="98" spans="1:9" ht="15.75">
       <c r="A98" s="17"/>
       <c r="B98" s="17" t="s">
         <v>21</v>
@@ -12975,7 +12975,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6">
+    <row r="99" spans="1:9" ht="15.75">
       <c r="A99" s="17" t="b">
         <v>0</v>
       </c>
@@ -12994,7 +12994,7 @@
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
     </row>
-    <row r="100" spans="1:9" ht="15.6">
+    <row r="100" spans="1:9" ht="15.75">
       <c r="A100" s="17"/>
       <c r="B100" s="17" t="s">
         <v>21</v>
@@ -13015,7 +13015,7 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
     </row>
-    <row r="101" spans="1:9" ht="15.6">
+    <row r="101" spans="1:9" ht="15.75">
       <c r="A101" s="17"/>
       <c r="B101" s="17" t="s">
         <v>21</v>
@@ -13040,7 +13040,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6">
+    <row r="102" spans="1:9" ht="15.75">
       <c r="A102" s="17" t="b">
         <v>0</v>
       </c>
@@ -13059,7 +13059,7 @@
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
     </row>
-    <row r="103" spans="1:9" ht="15.6">
+    <row r="103" spans="1:9" ht="15.75">
       <c r="A103" s="17"/>
       <c r="B103" s="17" t="s">
         <v>21</v>
@@ -13082,7 +13082,7 @@
       </c>
       <c r="I103" s="17"/>
     </row>
-    <row r="104" spans="1:9" ht="15.6">
+    <row r="104" spans="1:9" ht="15.75">
       <c r="A104" s="17"/>
       <c r="B104" s="17" t="s">
         <v>21</v>
@@ -13107,7 +13107,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6">
+    <row r="105" spans="1:9" ht="15.75">
       <c r="A105" s="17"/>
       <c r="B105" s="17" t="s">
         <v>21</v>
@@ -13130,7 +13130,7 @@
       </c>
       <c r="I105" s="17"/>
     </row>
-    <row r="106" spans="1:9" ht="15.6">
+    <row r="106" spans="1:9" ht="15.75">
       <c r="A106" s="17"/>
       <c r="B106" s="17" t="s">
         <v>21</v>
@@ -13151,7 +13151,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
     </row>
-    <row r="107" spans="1:9" ht="15.6">
+    <row r="107" spans="1:9" ht="15.75">
       <c r="A107" s="17" t="b">
         <v>0</v>
       </c>
@@ -13170,7 +13170,7 @@
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
     </row>
-    <row r="108" spans="1:9" ht="15.6">
+    <row r="108" spans="1:9" ht="15.75">
       <c r="A108" s="17"/>
       <c r="B108" s="17" t="s">
         <v>21</v>
@@ -13195,7 +13195,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6">
+    <row r="109" spans="1:9" ht="15.75">
       <c r="A109" s="17"/>
       <c r="B109" s="17" t="s">
         <v>21</v>
@@ -13218,7 +13218,7 @@
       </c>
       <c r="I109" s="17"/>
     </row>
-    <row r="110" spans="1:9" ht="15.6">
+    <row r="110" spans="1:9" ht="15.75">
       <c r="A110" s="17"/>
       <c r="B110" s="17" t="s">
         <v>21</v>
@@ -13241,7 +13241,7 @@
       </c>
       <c r="I110" s="17"/>
     </row>
-    <row r="111" spans="1:9" ht="15.6">
+    <row r="111" spans="1:9" ht="15.75">
       <c r="A111" s="17"/>
       <c r="B111" s="17" t="s">
         <v>21</v>
@@ -13264,7 +13264,7 @@
       </c>
       <c r="I111" s="17"/>
     </row>
-    <row r="112" spans="1:9" ht="15.6">
+    <row r="112" spans="1:9" ht="15.75">
       <c r="A112" s="17"/>
       <c r="B112" s="17" t="s">
         <v>21</v>
@@ -13287,7 +13287,7 @@
       </c>
       <c r="I112" s="17"/>
     </row>
-    <row r="113" spans="1:9" ht="15.6">
+    <row r="113" spans="1:9" ht="15.75">
       <c r="A113" s="17"/>
       <c r="B113" s="17" t="s">
         <v>21</v>
@@ -13310,7 +13310,7 @@
       </c>
       <c r="I113" s="17"/>
     </row>
-    <row r="114" spans="1:9" ht="15.6">
+    <row r="114" spans="1:9" ht="15.75">
       <c r="A114" s="17"/>
       <c r="B114" s="17" t="s">
         <v>21</v>
@@ -13333,7 +13333,7 @@
       </c>
       <c r="I114" s="17"/>
     </row>
-    <row r="115" spans="1:9" ht="15.6">
+    <row r="115" spans="1:9" ht="15.75">
       <c r="A115" s="17" t="b">
         <v>0</v>
       </c>
@@ -13352,7 +13352,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
     </row>
-    <row r="116" spans="1:9" ht="15.6">
+    <row r="116" spans="1:9" ht="15.75">
       <c r="A116" s="17"/>
       <c r="B116" s="17" t="s">
         <v>21</v>
@@ -13375,7 +13375,7 @@
       </c>
       <c r="I116" s="17"/>
     </row>
-    <row r="117" spans="1:9" ht="15.6">
+    <row r="117" spans="1:9" ht="15.75">
       <c r="A117" s="17"/>
       <c r="B117" s="17" t="s">
         <v>21</v>
@@ -13398,7 +13398,7 @@
       </c>
       <c r="I117" s="17"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6">
+    <row r="118" spans="1:9" ht="15.75">
       <c r="A118" s="17"/>
       <c r="B118" s="17" t="s">
         <v>21</v>
@@ -13421,7 +13421,7 @@
       </c>
       <c r="I118" s="17"/>
     </row>
-    <row r="119" spans="1:9" ht="15.6">
+    <row r="119" spans="1:9" ht="15.75">
       <c r="A119" s="17" t="b">
         <v>0</v>
       </c>
@@ -13440,7 +13440,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
     </row>
-    <row r="120" spans="1:9" ht="15.6">
+    <row r="120" spans="1:9" ht="15.75">
       <c r="A120" s="17"/>
       <c r="B120" s="17" t="s">
         <v>21</v>
@@ -13463,7 +13463,7 @@
       </c>
       <c r="I120" s="17"/>
     </row>
-    <row r="121" spans="1:9" ht="15.6">
+    <row r="121" spans="1:9" ht="15.75">
       <c r="A121" s="17"/>
       <c r="B121" s="17" t="s">
         <v>21</v>
@@ -13486,7 +13486,7 @@
       </c>
       <c r="I121" s="17"/>
     </row>
-    <row r="122" spans="1:9" ht="15.6">
+    <row r="122" spans="1:9" ht="15.75">
       <c r="A122" s="17"/>
       <c r="B122" s="17" t="s">
         <v>21</v>
@@ -13509,7 +13509,7 @@
       </c>
       <c r="I122" s="17"/>
     </row>
-    <row r="123" spans="1:9" ht="15.6">
+    <row r="123" spans="1:9" ht="15.75">
       <c r="A123" s="17"/>
       <c r="B123" s="17" t="s">
         <v>21</v>
@@ -13532,7 +13532,7 @@
       </c>
       <c r="I123" s="17"/>
     </row>
-    <row r="124" spans="1:9" ht="15.6">
+    <row r="124" spans="1:9" ht="15.75">
       <c r="A124" s="17"/>
       <c r="B124" s="17" t="s">
         <v>21</v>
@@ -13555,7 +13555,7 @@
       </c>
       <c r="I124" s="17"/>
     </row>
-    <row r="125" spans="1:9" ht="15.6">
+    <row r="125" spans="1:9" ht="15.75">
       <c r="A125" s="17"/>
       <c r="B125" s="17" t="s">
         <v>21</v>
@@ -13578,7 +13578,7 @@
       </c>
       <c r="I125" s="17"/>
     </row>
-    <row r="126" spans="1:9" ht="15.6">
+    <row r="126" spans="1:9" ht="15.75">
       <c r="A126" s="17" t="b">
         <v>0</v>
       </c>
@@ -13597,7 +13597,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
     </row>
-    <row r="127" spans="1:9" ht="15.6">
+    <row r="127" spans="1:9" ht="15.75">
       <c r="A127" s="17"/>
       <c r="B127" s="17" t="s">
         <v>21</v>
@@ -13622,7 +13622,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6">
+    <row r="128" spans="1:9" ht="15.75">
       <c r="A128" s="17"/>
       <c r="B128" s="17" t="s">
         <v>21</v>
@@ -13645,7 +13645,7 @@
       </c>
       <c r="I128" s="17"/>
     </row>
-    <row r="129" spans="1:9" ht="15.6">
+    <row r="129" spans="1:9" ht="15.75">
       <c r="A129" s="17"/>
       <c r="B129" s="17" t="s">
         <v>21</v>
@@ -13668,7 +13668,7 @@
       </c>
       <c r="I129" s="17"/>
     </row>
-    <row r="130" spans="1:9" ht="15.6">
+    <row r="130" spans="1:9" ht="15.75">
       <c r="A130" s="17"/>
       <c r="B130" s="17" t="s">
         <v>21</v>
@@ -13691,7 +13691,7 @@
       </c>
       <c r="I130" s="17"/>
     </row>
-    <row r="131" spans="1:9" ht="15.6">
+    <row r="131" spans="1:9" ht="15.75">
       <c r="A131" s="17"/>
       <c r="B131" s="17" t="s">
         <v>21</v>
@@ -13714,7 +13714,7 @@
       </c>
       <c r="I131" s="17"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6">
+    <row r="132" spans="1:9" ht="15.75">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>21</v>
@@ -13737,7 +13737,7 @@
       </c>
       <c r="I132" s="17"/>
     </row>
-    <row r="133" spans="1:9" ht="15.6">
+    <row r="133" spans="1:9" ht="15.75">
       <c r="A133" s="17"/>
       <c r="B133" s="17" t="s">
         <v>21</v>
@@ -13760,7 +13760,7 @@
       </c>
       <c r="I133" s="17"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6">
+    <row r="134" spans="1:9" ht="15.75">
       <c r="A134" s="17"/>
       <c r="B134" s="17" t="s">
         <v>21</v>
@@ -13783,7 +13783,7 @@
       </c>
       <c r="I134" s="17"/>
     </row>
-    <row r="135" spans="1:9" ht="15.6">
+    <row r="135" spans="1:9" ht="15.75">
       <c r="A135" s="17"/>
       <c r="B135" s="17" t="s">
         <v>21</v>
@@ -13806,7 +13806,7 @@
       </c>
       <c r="I135" s="17"/>
     </row>
-    <row r="136" spans="1:9" ht="15.6">
+    <row r="136" spans="1:9" ht="15.75">
       <c r="A136" s="17" t="b">
         <v>0</v>
       </c>
@@ -13825,7 +13825,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6">
+    <row r="137" spans="1:9" ht="15.75">
       <c r="A137" s="17"/>
       <c r="B137" s="17" t="s">
         <v>21</v>
@@ -13850,7 +13850,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6">
+    <row r="138" spans="1:9" ht="15.75">
       <c r="A138" s="17"/>
       <c r="B138" s="17" t="s">
         <v>21</v>
@@ -13871,7 +13871,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
     </row>
-    <row r="139" spans="1:9" ht="15.6">
+    <row r="139" spans="1:9" ht="15.75">
       <c r="A139" s="17"/>
       <c r="B139" s="17" t="s">
         <v>21</v>
@@ -13894,7 +13894,7 @@
       </c>
       <c r="I139" s="17"/>
     </row>
-    <row r="140" spans="1:9" ht="15.6">
+    <row r="140" spans="1:9" ht="15.75">
       <c r="A140" s="17"/>
       <c r="B140" s="17" t="s">
         <v>21</v>
@@ -13917,7 +13917,7 @@
       </c>
       <c r="I140" s="17"/>
     </row>
-    <row r="141" spans="1:9" ht="15.6">
+    <row r="141" spans="1:9" ht="15.75">
       <c r="A141" s="17"/>
       <c r="B141" s="17" t="s">
         <v>21</v>
@@ -13940,7 +13940,7 @@
       </c>
       <c r="I141" s="17"/>
     </row>
-    <row r="142" spans="1:9" ht="15.6">
+    <row r="142" spans="1:9" ht="15.75">
       <c r="A142" s="17"/>
       <c r="B142" s="17" t="s">
         <v>21</v>
@@ -13963,7 +13963,7 @@
       </c>
       <c r="I142" s="17"/>
     </row>
-    <row r="143" spans="1:9" ht="15.6">
+    <row r="143" spans="1:9" ht="15.75">
       <c r="A143" s="17"/>
       <c r="B143" s="17" t="s">
         <v>21</v>
@@ -13986,7 +13986,7 @@
       </c>
       <c r="I143" s="17"/>
     </row>
-    <row r="144" spans="1:9" ht="15.6">
+    <row r="144" spans="1:9" ht="15.75">
       <c r="A144" s="17"/>
       <c r="B144" s="17" t="s">
         <v>21</v>
@@ -14009,7 +14009,7 @@
       </c>
       <c r="I144" s="17"/>
     </row>
-    <row r="145" spans="1:9" ht="15.6">
+    <row r="145" spans="1:9" ht="15.75">
       <c r="A145" s="17"/>
       <c r="B145" s="17" t="s">
         <v>21</v>
@@ -14032,7 +14032,7 @@
       </c>
       <c r="I145" s="17"/>
     </row>
-    <row r="146" spans="1:9" ht="15.6">
+    <row r="146" spans="1:9" ht="15.75">
       <c r="A146" s="17"/>
       <c r="B146" s="17" t="s">
         <v>21</v>
@@ -14055,7 +14055,7 @@
       </c>
       <c r="I146" s="17"/>
     </row>
-    <row r="147" spans="1:9" ht="15.6">
+    <row r="147" spans="1:9" ht="15.75">
       <c r="A147" s="17"/>
       <c r="B147" s="17" t="s">
         <v>21</v>
@@ -14078,7 +14078,7 @@
       </c>
       <c r="I147" s="17"/>
     </row>
-    <row r="148" spans="1:9" ht="15.6">
+    <row r="148" spans="1:9" ht="15.75">
       <c r="A148" s="17"/>
       <c r="B148" s="17" t="s">
         <v>21</v>
@@ -14101,7 +14101,7 @@
       </c>
       <c r="I148" s="17"/>
     </row>
-    <row r="149" spans="1:9" ht="15.6">
+    <row r="149" spans="1:9" ht="15.75">
       <c r="A149" s="17"/>
       <c r="B149" s="17" t="s">
         <v>21</v>
@@ -14124,7 +14124,7 @@
       </c>
       <c r="I149" s="17"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6">
+    <row r="150" spans="1:9" ht="15.75">
       <c r="A150" s="17"/>
       <c r="B150" s="17" t="s">
         <v>21</v>
@@ -14147,7 +14147,7 @@
       </c>
       <c r="I150" s="17"/>
     </row>
-    <row r="151" spans="1:9" ht="15.6">
+    <row r="151" spans="1:9" ht="15.75">
       <c r="A151" s="17" t="b">
         <v>0</v>
       </c>
@@ -14166,7 +14166,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6">
+    <row r="152" spans="1:9" ht="15.75">
       <c r="A152" s="17"/>
       <c r="B152" s="17" t="s">
         <v>21</v>
@@ -14189,7 +14189,7 @@
       </c>
       <c r="I152" s="17"/>
     </row>
-    <row r="153" spans="1:9" ht="15.6">
+    <row r="153" spans="1:9" ht="15.75">
       <c r="A153" s="17" t="b">
         <v>0</v>
       </c>
@@ -14208,7 +14208,7 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
     </row>
-    <row r="154" spans="1:9" ht="15.6">
+    <row r="154" spans="1:9" ht="15.75">
       <c r="A154" s="17"/>
       <c r="B154" s="17" t="s">
         <v>21</v>
@@ -14231,7 +14231,7 @@
       </c>
       <c r="I154" s="17"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6">
+    <row r="155" spans="1:9" ht="15.75">
       <c r="A155" s="17"/>
       <c r="B155" s="17" t="s">
         <v>21</v>
@@ -14254,7 +14254,7 @@
       </c>
       <c r="I155" s="17"/>
     </row>
-    <row r="156" spans="1:9" ht="15.6">
+    <row r="156" spans="1:9" ht="15.75">
       <c r="A156" s="17" t="b">
         <v>0</v>
       </c>
@@ -14273,7 +14273,7 @@
       <c r="H156" s="17"/>
       <c r="I156" s="17"/>
     </row>
-    <row r="157" spans="1:9" ht="15.6">
+    <row r="157" spans="1:9" ht="15.75">
       <c r="A157" s="17"/>
       <c r="B157" s="17" t="s">
         <v>21</v>
@@ -14298,7 +14298,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6">
+    <row r="158" spans="1:9" ht="15.75">
       <c r="A158" s="17"/>
       <c r="B158" s="17" t="s">
         <v>21</v>
@@ -14321,7 +14321,7 @@
       </c>
       <c r="I158" s="17"/>
     </row>
-    <row r="159" spans="1:9" ht="15.6">
+    <row r="159" spans="1:9" ht="15.75">
       <c r="A159" s="17"/>
       <c r="B159" s="17" t="s">
         <v>21</v>
@@ -14344,7 +14344,7 @@
       </c>
       <c r="I159" s="17"/>
     </row>
-    <row r="160" spans="1:9" ht="15.6">
+    <row r="160" spans="1:9" ht="15.75">
       <c r="A160" s="17"/>
       <c r="B160" s="17" t="s">
         <v>21</v>
@@ -14367,7 +14367,7 @@
       </c>
       <c r="I160" s="17"/>
     </row>
-    <row r="161" spans="1:9" ht="15.6">
+    <row r="161" spans="1:9" ht="15.75">
       <c r="A161" s="17"/>
       <c r="B161" s="17" t="s">
         <v>21</v>
@@ -14390,7 +14390,7 @@
       </c>
       <c r="I161" s="17"/>
     </row>
-    <row r="162" spans="1:9" ht="15.6">
+    <row r="162" spans="1:9" ht="15.75">
       <c r="A162" s="17"/>
       <c r="B162" s="17" t="s">
         <v>21</v>
@@ -14413,7 +14413,7 @@
       </c>
       <c r="I162" s="17"/>
     </row>
-    <row r="163" spans="1:9" ht="15.6">
+    <row r="163" spans="1:9" ht="15.75">
       <c r="A163" s="17"/>
       <c r="B163" s="17" t="s">
         <v>21</v>
@@ -14436,7 +14436,7 @@
       </c>
       <c r="I163" s="17"/>
     </row>
-    <row r="164" spans="1:9" ht="15.6">
+    <row r="164" spans="1:9" ht="15.75">
       <c r="A164" s="17"/>
       <c r="B164" s="17" t="s">
         <v>21</v>
@@ -14459,7 +14459,7 @@
       </c>
       <c r="I164" s="17"/>
     </row>
-    <row r="165" spans="1:9" ht="15.6">
+    <row r="165" spans="1:9" ht="15.75">
       <c r="A165" s="17"/>
       <c r="B165" s="17" t="s">
         <v>21</v>
@@ -14482,7 +14482,7 @@
       </c>
       <c r="I165" s="17"/>
     </row>
-    <row r="166" spans="1:9" ht="15.6">
+    <row r="166" spans="1:9" ht="15.75">
       <c r="A166" s="17"/>
       <c r="B166" s="17" t="s">
         <v>21</v>
@@ -14505,7 +14505,7 @@
       </c>
       <c r="I166" s="17"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6">
+    <row r="167" spans="1:9" ht="15.75">
       <c r="A167" s="17" t="b">
         <v>0</v>
       </c>
@@ -14524,7 +14524,7 @@
       <c r="H167" s="17"/>
       <c r="I167" s="17"/>
     </row>
-    <row r="168" spans="1:9" ht="15.6">
+    <row r="168" spans="1:9" ht="15.75">
       <c r="A168" s="17"/>
       <c r="B168" s="17" t="s">
         <v>21</v>
@@ -14549,7 +14549,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6">
+    <row r="169" spans="1:9" ht="15.75">
       <c r="A169" s="17"/>
       <c r="B169" s="17" t="s">
         <v>21</v>
@@ -14572,7 +14572,7 @@
       </c>
       <c r="I169" s="17"/>
     </row>
-    <row r="170" spans="1:9" ht="15.6">
+    <row r="170" spans="1:9" ht="15.75">
       <c r="A170" s="17"/>
       <c r="B170" s="17" t="s">
         <v>21</v>
@@ -14595,7 +14595,7 @@
       </c>
       <c r="I170" s="17"/>
     </row>
-    <row r="171" spans="1:9" ht="15.6">
+    <row r="171" spans="1:9" ht="15.75">
       <c r="A171" s="17"/>
       <c r="B171" s="17" t="s">
         <v>21</v>
@@ -14618,7 +14618,7 @@
       </c>
       <c r="I171" s="17"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6">
+    <row r="172" spans="1:9" ht="15.75">
       <c r="A172" s="17"/>
       <c r="B172" s="17" t="s">
         <v>21</v>
@@ -14641,7 +14641,7 @@
       </c>
       <c r="I172" s="17"/>
     </row>
-    <row r="173" spans="1:9" ht="15.6">
+    <row r="173" spans="1:9" ht="15.75">
       <c r="A173" s="17"/>
       <c r="B173" s="17" t="s">
         <v>21</v>
@@ -14664,7 +14664,7 @@
       </c>
       <c r="I173" s="17"/>
     </row>
-    <row r="174" spans="1:9" ht="15.6">
+    <row r="174" spans="1:9" ht="15.75">
       <c r="A174" s="17"/>
       <c r="B174" s="17" t="s">
         <v>21</v>
@@ -14687,7 +14687,7 @@
       </c>
       <c r="I174" s="17"/>
     </row>
-    <row r="175" spans="1:9" ht="15.6">
+    <row r="175" spans="1:9" ht="15.75">
       <c r="A175" s="17"/>
       <c r="B175" s="17" t="s">
         <v>21</v>
@@ -14710,7 +14710,7 @@
       </c>
       <c r="I175" s="17"/>
     </row>
-    <row r="176" spans="1:9" ht="15.6">
+    <row r="176" spans="1:9" ht="15.75">
       <c r="A176" s="17"/>
       <c r="B176" s="17" t="s">
         <v>21</v>
@@ -14733,7 +14733,7 @@
       </c>
       <c r="I176" s="17"/>
     </row>
-    <row r="177" spans="1:9" ht="15.6">
+    <row r="177" spans="1:9" ht="15.75">
       <c r="A177" s="17"/>
       <c r="B177" s="17" t="s">
         <v>21</v>
@@ -14756,7 +14756,7 @@
       </c>
       <c r="I177" s="17"/>
     </row>
-    <row r="178" spans="1:9" ht="15.6">
+    <row r="178" spans="1:9" ht="15.75">
       <c r="A178" s="17" t="b">
         <v>0</v>
       </c>
@@ -14775,7 +14775,7 @@
       <c r="H178" s="17"/>
       <c r="I178" s="17"/>
     </row>
-    <row r="179" spans="1:9" ht="15.6">
+    <row r="179" spans="1:9" ht="15.75">
       <c r="A179" s="17"/>
       <c r="B179" s="17" t="s">
         <v>21</v>
@@ -14798,7 +14798,7 @@
       </c>
       <c r="I179" s="17"/>
     </row>
-    <row r="180" spans="1:9" ht="15.6">
+    <row r="180" spans="1:9" ht="15.75">
       <c r="A180" s="17"/>
       <c r="B180" s="17" t="s">
         <v>21</v>
@@ -14821,7 +14821,7 @@
       </c>
       <c r="I180" s="17"/>
     </row>
-    <row r="181" spans="1:9" ht="15.6">
+    <row r="181" spans="1:9" ht="15.75">
       <c r="A181" s="17"/>
       <c r="B181" s="17" t="s">
         <v>21</v>
@@ -14844,7 +14844,7 @@
       </c>
       <c r="I181" s="17"/>
     </row>
-    <row r="182" spans="1:9" ht="15.6">
+    <row r="182" spans="1:9" ht="15.75">
       <c r="A182" s="17"/>
       <c r="B182" s="17" t="s">
         <v>21</v>
@@ -14867,7 +14867,7 @@
       </c>
       <c r="I182" s="17"/>
     </row>
-    <row r="183" spans="1:9" ht="15.6">
+    <row r="183" spans="1:9" ht="15.75">
       <c r="A183" s="17" t="b">
         <v>0</v>
       </c>
@@ -14886,7 +14886,7 @@
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
     </row>
-    <row r="184" spans="1:9" ht="15.6">
+    <row r="184" spans="1:9" ht="15.75">
       <c r="A184" s="17"/>
       <c r="B184" s="17" t="s">
         <v>21</v>
@@ -14909,7 +14909,7 @@
       </c>
       <c r="I184" s="17"/>
     </row>
-    <row r="185" spans="1:9" ht="15.6">
+    <row r="185" spans="1:9" ht="15.75">
       <c r="A185" s="17"/>
       <c r="B185" s="17" t="s">
         <v>21</v>
@@ -14932,7 +14932,7 @@
       </c>
       <c r="I185" s="17"/>
     </row>
-    <row r="186" spans="1:9" ht="15.6">
+    <row r="186" spans="1:9" ht="15.75">
       <c r="A186" s="17"/>
       <c r="B186" s="17" t="s">
         <v>21</v>
@@ -14955,7 +14955,7 @@
       </c>
       <c r="I186" s="17"/>
     </row>
-    <row r="187" spans="1:9" ht="15.6">
+    <row r="187" spans="1:9" ht="15.75">
       <c r="A187" s="17"/>
       <c r="B187" s="17" t="s">
         <v>21</v>
@@ -14978,7 +14978,7 @@
       </c>
       <c r="I187" s="17"/>
     </row>
-    <row r="188" spans="1:9" ht="15.6">
+    <row r="188" spans="1:9" ht="15.75">
       <c r="A188" s="17" t="b">
         <v>0</v>
       </c>
@@ -14997,7 +14997,7 @@
       <c r="H188" s="17"/>
       <c r="I188" s="17"/>
     </row>
-    <row r="189" spans="1:9" ht="15.6">
+    <row r="189" spans="1:9" ht="15.75">
       <c r="A189" s="17"/>
       <c r="B189" s="17" t="s">
         <v>21</v>
@@ -15018,7 +15018,7 @@
       <c r="H189" s="17"/>
       <c r="I189" s="17"/>
     </row>
-    <row r="190" spans="1:9" ht="15.6">
+    <row r="190" spans="1:9" ht="15.75">
       <c r="A190" s="17"/>
       <c r="B190" s="17" t="s">
         <v>21</v>
@@ -15041,7 +15041,7 @@
       </c>
       <c r="I190" s="17"/>
     </row>
-    <row r="191" spans="1:9" ht="15.6">
+    <row r="191" spans="1:9" ht="15.75">
       <c r="A191" s="17" t="b">
         <v>0</v>
       </c>
@@ -15060,7 +15060,7 @@
       <c r="H191" s="17"/>
       <c r="I191" s="17"/>
     </row>
-    <row r="192" spans="1:9" ht="15.6">
+    <row r="192" spans="1:9" ht="15.75">
       <c r="A192" s="17"/>
       <c r="B192" s="17" t="s">
         <v>21</v>
@@ -15083,7 +15083,7 @@
       </c>
       <c r="I192" s="17"/>
     </row>
-    <row r="193" spans="1:9" ht="15.6">
+    <row r="193" spans="1:9" ht="15.75">
       <c r="A193" s="17"/>
       <c r="B193" s="17" t="s">
         <v>21</v>
@@ -15108,7 +15108,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6">
+    <row r="194" spans="1:9" ht="15.75">
       <c r="A194" s="17"/>
       <c r="B194" s="17" t="s">
         <v>21</v>
@@ -15129,7 +15129,7 @@
       <c r="H194" s="17"/>
       <c r="I194" s="17"/>
     </row>
-    <row r="195" spans="1:9" ht="15.6">
+    <row r="195" spans="1:9" ht="15.75">
       <c r="A195" s="17"/>
       <c r="B195" s="17" t="s">
         <v>21</v>
@@ -15154,7 +15154,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6">
+    <row r="196" spans="1:9" ht="15.75">
       <c r="A196" s="17"/>
       <c r="B196" s="17" t="s">
         <v>21</v>
@@ -15179,7 +15179,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6">
+    <row r="197" spans="1:9" ht="15.75">
       <c r="A197" s="17" t="b">
         <v>0</v>
       </c>
@@ -15198,7 +15198,7 @@
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
     </row>
-    <row r="198" spans="1:9" ht="15.6">
+    <row r="198" spans="1:9" ht="15.75">
       <c r="A198" s="17"/>
       <c r="B198" s="17" t="s">
         <v>21</v>
@@ -15223,7 +15223,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6">
+    <row r="199" spans="1:9" ht="15.75">
       <c r="A199" s="17"/>
       <c r="B199" s="17" t="s">
         <v>21</v>
@@ -15246,7 +15246,7 @@
       </c>
       <c r="I199" s="17"/>
     </row>
-    <row r="200" spans="1:9" ht="15.6">
+    <row r="200" spans="1:9" ht="15.75">
       <c r="A200" s="17"/>
       <c r="B200" s="17" t="s">
         <v>21</v>
@@ -15269,7 +15269,7 @@
       </c>
       <c r="I200" s="17"/>
     </row>
-    <row r="201" spans="1:9" ht="15.6">
+    <row r="201" spans="1:9" ht="15.75">
       <c r="A201" s="17"/>
       <c r="B201" s="17" t="s">
         <v>21</v>
@@ -15292,7 +15292,7 @@
       </c>
       <c r="I201" s="17"/>
     </row>
-    <row r="202" spans="1:9" ht="15.6">
+    <row r="202" spans="1:9" ht="15.75">
       <c r="A202" s="17"/>
       <c r="B202" s="17" t="s">
         <v>21</v>
@@ -15315,7 +15315,7 @@
       </c>
       <c r="I202" s="17"/>
     </row>
-    <row r="203" spans="1:9" ht="15.6">
+    <row r="203" spans="1:9" ht="15.75">
       <c r="A203" s="17"/>
       <c r="B203" s="17" t="s">
         <v>21</v>
@@ -15338,7 +15338,7 @@
       </c>
       <c r="I203" s="17"/>
     </row>
-    <row r="204" spans="1:9" ht="15.6">
+    <row r="204" spans="1:9" ht="15.75">
       <c r="A204" s="17"/>
       <c r="B204" s="17" t="s">
         <v>21</v>
@@ -15361,7 +15361,7 @@
       </c>
       <c r="I204" s="17"/>
     </row>
-    <row r="205" spans="1:9" ht="15.6">
+    <row r="205" spans="1:9" ht="15.75">
       <c r="A205" s="17"/>
       <c r="B205" s="17" t="s">
         <v>21</v>
@@ -15384,7 +15384,7 @@
       </c>
       <c r="I205" s="17"/>
     </row>
-    <row r="206" spans="1:9" ht="15.6">
+    <row r="206" spans="1:9" ht="15.75">
       <c r="A206" s="17"/>
       <c r="B206" s="17" t="s">
         <v>21</v>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="I206" s="17"/>
     </row>
-    <row r="207" spans="1:9" ht="15.6">
+    <row r="207" spans="1:9" ht="15.75">
       <c r="A207" s="17" t="b">
         <v>0</v>
       </c>
@@ -15426,7 +15426,7 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
     </row>
-    <row r="208" spans="1:9" ht="15.6">
+    <row r="208" spans="1:9" ht="15.75">
       <c r="A208" s="17"/>
       <c r="B208" s="17" t="s">
         <v>21</v>
@@ -15451,7 +15451,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6">
+    <row r="209" spans="1:9" ht="15.75">
       <c r="A209" s="17"/>
       <c r="B209" s="17" t="s">
         <v>21</v>
@@ -15474,7 +15474,7 @@
       </c>
       <c r="I209" s="17"/>
     </row>
-    <row r="210" spans="1:9" ht="15.6">
+    <row r="210" spans="1:9" ht="15.75">
       <c r="A210" s="17"/>
       <c r="B210" s="17" t="s">
         <v>21</v>
@@ -15497,7 +15497,7 @@
       </c>
       <c r="I210" s="17"/>
     </row>
-    <row r="211" spans="1:9" ht="15.6">
+    <row r="211" spans="1:9" ht="15.75">
       <c r="A211" s="17"/>
       <c r="B211" s="17" t="s">
         <v>21</v>
@@ -15520,7 +15520,7 @@
       </c>
       <c r="I211" s="17"/>
     </row>
-    <row r="212" spans="1:9" ht="15.6">
+    <row r="212" spans="1:9" ht="15.75">
       <c r="A212" s="17"/>
       <c r="B212" s="17" t="s">
         <v>21</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="I212" s="17"/>
     </row>
-    <row r="213" spans="1:9" ht="15.6">
+    <row r="213" spans="1:9" ht="15.75">
       <c r="A213" s="17"/>
       <c r="B213" s="17" t="s">
         <v>21</v>
@@ -15566,7 +15566,7 @@
       </c>
       <c r="I213" s="17"/>
     </row>
-    <row r="214" spans="1:9" ht="15.6">
+    <row r="214" spans="1:9" ht="15.75">
       <c r="A214" s="17"/>
       <c r="B214" s="17" t="s">
         <v>21</v>
@@ -15589,7 +15589,7 @@
       </c>
       <c r="I214" s="17"/>
     </row>
-    <row r="215" spans="1:9" ht="15.6">
+    <row r="215" spans="1:9" ht="15.75">
       <c r="A215" s="17"/>
       <c r="B215" s="17" t="s">
         <v>21</v>
@@ -15612,7 +15612,7 @@
       </c>
       <c r="I215" s="17"/>
     </row>
-    <row r="216" spans="1:9" ht="15.6">
+    <row r="216" spans="1:9" ht="15.75">
       <c r="A216" s="17"/>
       <c r="B216" s="17" t="s">
         <v>21</v>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="I216" s="17"/>
     </row>
-    <row r="217" spans="1:9" ht="15.6">
+    <row r="217" spans="1:9" ht="15.75">
       <c r="A217" s="17" t="b">
         <v>0</v>
       </c>
@@ -15654,7 +15654,7 @@
       <c r="H217" s="17"/>
       <c r="I217" s="17"/>
     </row>
-    <row r="218" spans="1:9" ht="15.6">
+    <row r="218" spans="1:9" ht="15.75">
       <c r="A218" s="17"/>
       <c r="B218" s="17" t="s">
         <v>21</v>
@@ -15675,7 +15675,7 @@
       <c r="H218" s="17"/>
       <c r="I218" s="17"/>
     </row>
-    <row r="219" spans="1:9" ht="15.6">
+    <row r="219" spans="1:9" ht="15.75">
       <c r="A219" s="17"/>
       <c r="B219" s="17" t="s">
         <v>21</v>
@@ -15698,7 +15698,7 @@
       </c>
       <c r="I219" s="17"/>
     </row>
-    <row r="220" spans="1:9" ht="15.6">
+    <row r="220" spans="1:9" ht="15.75">
       <c r="A220" s="17"/>
       <c r="B220" s="17" t="s">
         <v>21</v>
@@ -15721,7 +15721,7 @@
       </c>
       <c r="I220" s="17"/>
     </row>
-    <row r="221" spans="1:9" ht="15.6">
+    <row r="221" spans="1:9" ht="15.75">
       <c r="A221" s="17"/>
       <c r="B221" s="17" t="s">
         <v>21</v>
@@ -15744,7 +15744,7 @@
       </c>
       <c r="I221" s="17"/>
     </row>
-    <row r="222" spans="1:9" ht="15.6">
+    <row r="222" spans="1:9" ht="15.75">
       <c r="A222" s="17"/>
       <c r="B222" s="17" t="s">
         <v>21</v>
@@ -15767,7 +15767,7 @@
       </c>
       <c r="I222" s="17"/>
     </row>
-    <row r="223" spans="1:9" ht="15.6">
+    <row r="223" spans="1:9" ht="15.75">
       <c r="A223" s="17"/>
       <c r="B223" s="17" t="s">
         <v>21</v>
@@ -15790,7 +15790,7 @@
       </c>
       <c r="I223" s="17"/>
     </row>
-    <row r="224" spans="1:9" ht="15.6">
+    <row r="224" spans="1:9" ht="15.75">
       <c r="A224" s="17"/>
       <c r="B224" s="17" t="s">
         <v>21</v>
@@ -15813,7 +15813,7 @@
       </c>
       <c r="I224" s="17"/>
     </row>
-    <row r="225" spans="1:9" ht="15.6">
+    <row r="225" spans="1:9" ht="15.75">
       <c r="A225" s="17"/>
       <c r="B225" s="17" t="s">
         <v>21</v>
@@ -15836,7 +15836,7 @@
       </c>
       <c r="I225" s="17"/>
     </row>
-    <row r="226" spans="1:9" ht="15.6">
+    <row r="226" spans="1:9" ht="15.75">
       <c r="A226" s="17"/>
       <c r="B226" s="17" t="s">
         <v>21</v>
@@ -15859,7 +15859,7 @@
       </c>
       <c r="I226" s="17"/>
     </row>
-    <row r="227" spans="1:9" ht="15.6">
+    <row r="227" spans="1:9" ht="15.75">
       <c r="A227" s="17"/>
       <c r="B227" s="17" t="s">
         <v>21</v>
@@ -15882,7 +15882,7 @@
       </c>
       <c r="I227" s="17"/>
     </row>
-    <row r="228" spans="1:9" ht="15.6">
+    <row r="228" spans="1:9" ht="15.75">
       <c r="A228" s="17"/>
       <c r="B228" s="17" t="s">
         <v>21</v>
@@ -15905,7 +15905,7 @@
       </c>
       <c r="I228" s="17"/>
     </row>
-    <row r="229" spans="1:9" ht="15.6">
+    <row r="229" spans="1:9" ht="15.75">
       <c r="A229" s="17"/>
       <c r="B229" s="17" t="s">
         <v>21</v>
@@ -15928,7 +15928,7 @@
       </c>
       <c r="I229" s="17"/>
     </row>
-    <row r="230" spans="1:9" ht="15.6">
+    <row r="230" spans="1:9" ht="15.75">
       <c r="A230" s="17"/>
       <c r="B230" s="17" t="s">
         <v>21</v>
@@ -15951,7 +15951,7 @@
       </c>
       <c r="I230" s="17"/>
     </row>
-    <row r="231" spans="1:9" ht="15.6">
+    <row r="231" spans="1:9" ht="15.75">
       <c r="A231" s="17"/>
       <c r="B231" s="17" t="s">
         <v>21</v>
@@ -15974,7 +15974,7 @@
       </c>
       <c r="I231" s="17"/>
     </row>
-    <row r="232" spans="1:9" ht="15.6">
+    <row r="232" spans="1:9" ht="15.75">
       <c r="A232" s="17"/>
       <c r="B232" s="17" t="s">
         <v>21</v>
@@ -15997,7 +15997,7 @@
       </c>
       <c r="I232" s="17"/>
     </row>
-    <row r="233" spans="1:9" ht="15.6">
+    <row r="233" spans="1:9" ht="15.75">
       <c r="A233" s="17"/>
       <c r="B233" s="17" t="s">
         <v>21</v>
@@ -16020,7 +16020,7 @@
       </c>
       <c r="I233" s="17"/>
     </row>
-    <row r="234" spans="1:9" ht="15.6">
+    <row r="234" spans="1:9" ht="15.75">
       <c r="A234" s="17" t="b">
         <v>0</v>
       </c>
@@ -16039,7 +16039,7 @@
       <c r="H234" s="17"/>
       <c r="I234" s="17"/>
     </row>
-    <row r="235" spans="1:9" ht="15.6">
+    <row r="235" spans="1:9" ht="15.75">
       <c r="A235" s="17"/>
       <c r="B235" s="17" t="s">
         <v>21</v>
@@ -16060,7 +16060,7 @@
       <c r="H235" s="17"/>
       <c r="I235" s="17"/>
     </row>
-    <row r="236" spans="1:9" ht="15.6">
+    <row r="236" spans="1:9" ht="15.75">
       <c r="A236" s="17"/>
       <c r="B236" s="17" t="s">
         <v>21</v>
@@ -16083,7 +16083,7 @@
       </c>
       <c r="I236" s="17"/>
     </row>
-    <row r="237" spans="1:9" ht="15.6">
+    <row r="237" spans="1:9" ht="15.75">
       <c r="A237" s="17"/>
       <c r="B237" s="17" t="s">
         <v>21</v>
@@ -16106,7 +16106,7 @@
       </c>
       <c r="I237" s="17"/>
     </row>
-    <row r="238" spans="1:9" ht="15.6">
+    <row r="238" spans="1:9" ht="15.75">
       <c r="A238" s="17"/>
       <c r="B238" s="17" t="s">
         <v>21</v>
@@ -16129,7 +16129,7 @@
       </c>
       <c r="I238" s="17"/>
     </row>
-    <row r="239" spans="1:9" ht="15.6">
+    <row r="239" spans="1:9" ht="15.75">
       <c r="A239" s="17"/>
       <c r="B239" s="17" t="s">
         <v>21</v>
@@ -16152,7 +16152,7 @@
       </c>
       <c r="I239" s="17"/>
     </row>
-    <row r="240" spans="1:9" ht="15.6">
+    <row r="240" spans="1:9" ht="15.75">
       <c r="A240" s="17"/>
       <c r="B240" s="17" t="s">
         <v>21</v>
@@ -16175,7 +16175,7 @@
       </c>
       <c r="I240" s="17"/>
     </row>
-    <row r="241" spans="1:9" ht="15.6">
+    <row r="241" spans="1:9" ht="15.75">
       <c r="A241" s="17"/>
       <c r="B241" s="17" t="s">
         <v>21</v>
@@ -16198,7 +16198,7 @@
       </c>
       <c r="I241" s="17"/>
     </row>
-    <row r="242" spans="1:9" ht="15.6">
+    <row r="242" spans="1:9" ht="15.75">
       <c r="A242" s="17"/>
       <c r="B242" s="17" t="s">
         <v>21</v>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="I242" s="17"/>
     </row>
-    <row r="243" spans="1:9" ht="15.6">
+    <row r="243" spans="1:9" ht="15.75">
       <c r="A243" s="17"/>
       <c r="B243" s="17" t="s">
         <v>21</v>
@@ -16244,7 +16244,7 @@
       </c>
       <c r="I243" s="17"/>
     </row>
-    <row r="244" spans="1:9" ht="15.6">
+    <row r="244" spans="1:9" ht="15.75">
       <c r="A244" s="17"/>
       <c r="B244" s="17" t="s">
         <v>21</v>
@@ -16267,7 +16267,7 @@
       </c>
       <c r="I244" s="17"/>
     </row>
-    <row r="245" spans="1:9" ht="15.6">
+    <row r="245" spans="1:9" ht="15.75">
       <c r="A245" s="17"/>
       <c r="B245" s="17" t="s">
         <v>21</v>
@@ -16290,7 +16290,7 @@
       </c>
       <c r="I245" s="17"/>
     </row>
-    <row r="246" spans="1:9" ht="15.6">
+    <row r="246" spans="1:9" ht="15.75">
       <c r="A246" s="17"/>
       <c r="B246" s="17" t="s">
         <v>21</v>
@@ -16313,7 +16313,7 @@
       </c>
       <c r="I246" s="17"/>
     </row>
-    <row r="247" spans="1:9" ht="15.6">
+    <row r="247" spans="1:9" ht="15.75">
       <c r="A247" s="17"/>
       <c r="B247" s="17" t="s">
         <v>21</v>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="I247" s="17"/>
     </row>
-    <row r="248" spans="1:9" ht="15.6">
+    <row r="248" spans="1:9" ht="15.75">
       <c r="A248" s="17"/>
       <c r="B248" s="17" t="s">
         <v>21</v>
@@ -16359,7 +16359,7 @@
       </c>
       <c r="I248" s="17"/>
     </row>
-    <row r="249" spans="1:9" ht="15.6">
+    <row r="249" spans="1:9" ht="15.75">
       <c r="A249" s="17"/>
       <c r="B249" s="17" t="s">
         <v>21</v>
@@ -16382,7 +16382,7 @@
       </c>
       <c r="I249" s="17"/>
     </row>
-    <row r="250" spans="1:9" ht="15.6">
+    <row r="250" spans="1:9" ht="15.75">
       <c r="A250" s="17"/>
       <c r="B250" s="17" t="s">
         <v>21</v>
@@ -16405,7 +16405,7 @@
       </c>
       <c r="I250" s="17"/>
     </row>
-    <row r="251" spans="1:9" ht="15.6">
+    <row r="251" spans="1:9" ht="15.75">
       <c r="A251" s="17" t="b">
         <v>0</v>
       </c>
@@ -16424,7 +16424,7 @@
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
     </row>
-    <row r="252" spans="1:9" ht="15.6">
+    <row r="252" spans="1:9" ht="15.75">
       <c r="A252" s="17"/>
       <c r="B252" s="17" t="s">
         <v>21</v>
@@ -16449,7 +16449,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.6">
+    <row r="253" spans="1:9" ht="15.75">
       <c r="A253" s="17"/>
       <c r="B253" s="17" t="s">
         <v>21</v>
@@ -16472,7 +16472,7 @@
       </c>
       <c r="I253" s="17"/>
     </row>
-    <row r="254" spans="1:9" ht="15.6">
+    <row r="254" spans="1:9" ht="15.75">
       <c r="A254" s="17"/>
       <c r="B254" s="17" t="s">
         <v>21</v>
@@ -16495,7 +16495,7 @@
       </c>
       <c r="I254" s="17"/>
     </row>
-    <row r="255" spans="1:9" ht="15.6">
+    <row r="255" spans="1:9" ht="15.75">
       <c r="A255" s="17"/>
       <c r="B255" s="17" t="s">
         <v>21</v>
@@ -16518,7 +16518,7 @@
       </c>
       <c r="I255" s="17"/>
     </row>
-    <row r="256" spans="1:9" ht="15.6">
+    <row r="256" spans="1:9" ht="15.75">
       <c r="A256" s="17"/>
       <c r="B256" s="17" t="s">
         <v>21</v>
@@ -16541,7 +16541,7 @@
       </c>
       <c r="I256" s="17"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6">
+    <row r="257" spans="1:9" ht="15.75">
       <c r="A257" s="17" t="b">
         <v>0</v>
       </c>
@@ -16560,7 +16560,7 @@
       <c r="H257" s="17"/>
       <c r="I257" s="17"/>
     </row>
-    <row r="258" spans="1:9" ht="15.6">
+    <row r="258" spans="1:9" ht="15.75">
       <c r="A258" s="17"/>
       <c r="B258" s="17" t="s">
         <v>21</v>
@@ -16585,7 +16585,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.6">
+    <row r="259" spans="1:9" ht="15.75">
       <c r="A259" s="17"/>
       <c r="B259" s="17" t="s">
         <v>21</v>
@@ -16608,7 +16608,7 @@
       </c>
       <c r="I259" s="17"/>
     </row>
-    <row r="260" spans="1:9" ht="15.6">
+    <row r="260" spans="1:9" ht="15.75">
       <c r="A260" s="17" t="b">
         <v>0</v>
       </c>
@@ -16627,7 +16627,7 @@
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
     </row>
-    <row r="261" spans="1:9" ht="15.6">
+    <row r="261" spans="1:9" ht="15.75">
       <c r="A261" s="17" t="b">
         <v>0</v>
       </c>
@@ -16646,7 +16646,7 @@
       <c r="H261" s="17"/>
       <c r="I261" s="17"/>
     </row>
-    <row r="262" spans="1:9" ht="15.6">
+    <row r="262" spans="1:9" ht="15.75">
       <c r="A262" s="17" t="b">
         <v>0</v>
       </c>
@@ -16665,7 +16665,7 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
     </row>
-    <row r="263" spans="1:9" ht="15.6">
+    <row r="263" spans="1:9" ht="15.75">
       <c r="A263" s="17"/>
       <c r="B263" s="17" t="s">
         <v>21</v>
@@ -16686,7 +16686,7 @@
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
     </row>
-    <row r="264" spans="1:9" ht="15.6">
+    <row r="264" spans="1:9" ht="15.75">
       <c r="A264" s="17"/>
       <c r="B264" s="17" t="s">
         <v>21</v>
@@ -16709,7 +16709,7 @@
       </c>
       <c r="I264" s="17"/>
     </row>
-    <row r="265" spans="1:9" ht="15.6">
+    <row r="265" spans="1:9" ht="15.75">
       <c r="A265" s="17"/>
       <c r="B265" s="17" t="s">
         <v>21</v>
@@ -16732,7 +16732,7 @@
       </c>
       <c r="I265" s="17"/>
     </row>
-    <row r="266" spans="1:9" ht="15.6">
+    <row r="266" spans="1:9" ht="15.75">
       <c r="A266" s="17"/>
       <c r="B266" s="17" t="s">
         <v>21</v>
@@ -16755,7 +16755,7 @@
       </c>
       <c r="I266" s="17"/>
     </row>
-    <row r="267" spans="1:9" ht="15.6">
+    <row r="267" spans="1:9" ht="15.75">
       <c r="A267" s="17"/>
       <c r="B267" s="17" t="s">
         <v>21</v>
@@ -16778,7 +16778,7 @@
       </c>
       <c r="I267" s="17"/>
     </row>
-    <row r="268" spans="1:9" ht="15.6">
+    <row r="268" spans="1:9" ht="15.75">
       <c r="A268" s="17"/>
       <c r="B268" s="17" t="s">
         <v>21</v>
@@ -16801,7 +16801,7 @@
       </c>
       <c r="I268" s="17"/>
     </row>
-    <row r="269" spans="1:9" ht="15.6">
+    <row r="269" spans="1:9" ht="15.75">
       <c r="A269" s="17"/>
       <c r="B269" s="17" t="s">
         <v>21</v>
@@ -16824,7 +16824,7 @@
       </c>
       <c r="I269" s="17"/>
     </row>
-    <row r="270" spans="1:9" ht="15.6">
+    <row r="270" spans="1:9" ht="15.75">
       <c r="A270" s="17"/>
       <c r="B270" s="17" t="s">
         <v>21</v>
@@ -16847,7 +16847,7 @@
       </c>
       <c r="I270" s="17"/>
     </row>
-    <row r="271" spans="1:9" ht="15.6">
+    <row r="271" spans="1:9" ht="15.75">
       <c r="A271" s="17"/>
       <c r="B271" s="17" t="s">
         <v>21</v>
@@ -16870,7 +16870,7 @@
       </c>
       <c r="I271" s="17"/>
     </row>
-    <row r="272" spans="1:9" ht="15.6">
+    <row r="272" spans="1:9" ht="15.75">
       <c r="A272" s="17"/>
       <c r="B272" s="17" t="s">
         <v>21</v>
@@ -16893,7 +16893,7 @@
       </c>
       <c r="I272" s="17"/>
     </row>
-    <row r="273" spans="1:9" ht="15.6">
+    <row r="273" spans="1:9" ht="15.75">
       <c r="A273" s="17"/>
       <c r="B273" s="17" t="s">
         <v>21</v>
@@ -16916,7 +16916,7 @@
       </c>
       <c r="I273" s="17"/>
     </row>
-    <row r="274" spans="1:9" ht="15.6">
+    <row r="274" spans="1:9" ht="15.75">
       <c r="A274" s="17" t="b">
         <v>0</v>
       </c>
@@ -16935,7 +16935,7 @@
       <c r="H274" s="17"/>
       <c r="I274" s="17"/>
     </row>
-    <row r="275" spans="1:9" ht="15.6">
+    <row r="275" spans="1:9" ht="15.75">
       <c r="A275" s="17"/>
       <c r="B275" s="17" t="s">
         <v>21</v>
@@ -16958,7 +16958,7 @@
       </c>
       <c r="I275" s="17"/>
     </row>
-    <row r="276" spans="1:9" ht="15.6">
+    <row r="276" spans="1:9" ht="15.75">
       <c r="A276" s="17" t="b">
         <v>0</v>
       </c>
@@ -16977,7 +16977,7 @@
       <c r="H276" s="17"/>
       <c r="I276" s="17"/>
     </row>
-    <row r="277" spans="1:9" ht="15.6">
+    <row r="277" spans="1:9" ht="15.75">
       <c r="A277" s="17"/>
       <c r="B277" s="17" t="s">
         <v>21</v>
@@ -17002,7 +17002,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.6">
+    <row r="278" spans="1:9" ht="15.75">
       <c r="A278" s="17"/>
       <c r="B278" s="17" t="s">
         <v>21</v>
@@ -17025,7 +17025,7 @@
       </c>
       <c r="I278" s="17"/>
     </row>
-    <row r="279" spans="1:9" ht="15.6">
+    <row r="279" spans="1:9" ht="15.75">
       <c r="A279" s="17"/>
       <c r="B279" s="17" t="s">
         <v>21</v>
@@ -17048,7 +17048,7 @@
       </c>
       <c r="I279" s="17"/>
     </row>
-    <row r="280" spans="1:9" ht="15.6">
+    <row r="280" spans="1:9" ht="15.75">
       <c r="A280" s="17"/>
       <c r="B280" s="17" t="s">
         <v>21</v>
@@ -17071,7 +17071,7 @@
       </c>
       <c r="I280" s="17"/>
     </row>
-    <row r="281" spans="1:9" ht="15.6">
+    <row r="281" spans="1:9" ht="15.75">
       <c r="A281" s="17"/>
       <c r="B281" s="17" t="s">
         <v>21</v>
@@ -17094,7 +17094,7 @@
       </c>
       <c r="I281" s="17"/>
     </row>
-    <row r="282" spans="1:9" ht="15.6">
+    <row r="282" spans="1:9" ht="15.75">
       <c r="A282" s="17"/>
       <c r="B282" s="17" t="s">
         <v>21</v>
@@ -17117,7 +17117,7 @@
       </c>
       <c r="I282" s="17"/>
     </row>
-    <row r="283" spans="1:9" ht="15.6">
+    <row r="283" spans="1:9" ht="15.75">
       <c r="A283" s="17"/>
       <c r="B283" s="17" t="s">
         <v>21</v>
@@ -17140,7 +17140,7 @@
       </c>
       <c r="I283" s="17"/>
     </row>
-    <row r="284" spans="1:9" ht="15.6">
+    <row r="284" spans="1:9" ht="15.75">
       <c r="A284" s="17"/>
       <c r="B284" s="17" t="s">
         <v>21</v>
@@ -17163,7 +17163,7 @@
       </c>
       <c r="I284" s="17"/>
     </row>
-    <row r="285" spans="1:9" ht="15.6">
+    <row r="285" spans="1:9" ht="15.75">
       <c r="A285" s="17"/>
       <c r="B285" s="17" t="s">
         <v>21</v>
@@ -17186,7 +17186,7 @@
       </c>
       <c r="I285" s="17"/>
     </row>
-    <row r="286" spans="1:9" ht="15.6">
+    <row r="286" spans="1:9" ht="15.75">
       <c r="A286" s="17"/>
       <c r="B286" s="17" t="s">
         <v>21</v>
@@ -17209,7 +17209,7 @@
       </c>
       <c r="I286" s="17"/>
     </row>
-    <row r="287" spans="1:9" ht="15.6">
+    <row r="287" spans="1:9" ht="15.75">
       <c r="A287" s="17"/>
       <c r="B287" s="17" t="s">
         <v>21</v>
@@ -17232,7 +17232,7 @@
       </c>
       <c r="I287" s="17"/>
     </row>
-    <row r="288" spans="1:9" ht="15.6">
+    <row r="288" spans="1:9" ht="15.75">
       <c r="A288" s="17" t="b">
         <v>0</v>
       </c>
@@ -17251,7 +17251,7 @@
       <c r="H288" s="17"/>
       <c r="I288" s="17"/>
     </row>
-    <row r="289" spans="1:9" ht="15.6">
+    <row r="289" spans="1:9" ht="15.75">
       <c r="A289" s="17"/>
       <c r="B289" s="17" t="s">
         <v>21</v>
@@ -17274,7 +17274,7 @@
       </c>
       <c r="I289" s="17"/>
     </row>
-    <row r="290" spans="1:9" ht="15.6">
+    <row r="290" spans="1:9" ht="15.75">
       <c r="A290" s="17" t="b">
         <v>0</v>
       </c>
@@ -17293,7 +17293,7 @@
       <c r="H290" s="17"/>
       <c r="I290" s="17"/>
     </row>
-    <row r="291" spans="1:9" ht="15.6">
+    <row r="291" spans="1:9" ht="15.75">
       <c r="A291" s="17"/>
       <c r="B291" s="17" t="s">
         <v>21</v>
@@ -17314,7 +17314,7 @@
       <c r="H291" s="17"/>
       <c r="I291" s="17"/>
     </row>
-    <row r="292" spans="1:9" ht="15.6">
+    <row r="292" spans="1:9" ht="15.75">
       <c r="A292" s="17" t="b">
         <v>0</v>
       </c>
@@ -17333,7 +17333,7 @@
       <c r="H292" s="17"/>
       <c r="I292" s="17"/>
     </row>
-    <row r="293" spans="1:9" ht="15.6">
+    <row r="293" spans="1:9" ht="15.75">
       <c r="A293" s="17"/>
       <c r="B293" s="17" t="s">
         <v>21</v>
@@ -17354,7 +17354,7 @@
       <c r="H293" s="17"/>
       <c r="I293" s="17"/>
     </row>
-    <row r="294" spans="1:9" ht="15.6">
+    <row r="294" spans="1:9" ht="15.75">
       <c r="A294" s="17" t="b">
         <v>0</v>
       </c>
@@ -17373,7 +17373,7 @@
       <c r="H294" s="17"/>
       <c r="I294" s="17"/>
     </row>
-    <row r="295" spans="1:9" ht="15.6">
+    <row r="295" spans="1:9" ht="15.75">
       <c r="A295" s="17"/>
       <c r="B295" s="17" t="s">
         <v>21</v>
@@ -17394,7 +17394,7 @@
       <c r="H295" s="17"/>
       <c r="I295" s="17"/>
     </row>
-    <row r="296" spans="1:9" ht="15.6">
+    <row r="296" spans="1:9" ht="15.75">
       <c r="A296" s="17" t="b">
         <v>0</v>
       </c>
@@ -17413,7 +17413,7 @@
       <c r="H296" s="17"/>
       <c r="I296" s="17"/>
     </row>
-    <row r="297" spans="1:9" ht="15.6">
+    <row r="297" spans="1:9" ht="15.75">
       <c r="A297" s="17"/>
       <c r="B297" s="17" t="s">
         <v>21</v>
@@ -17436,7 +17436,7 @@
       </c>
       <c r="I297" s="17"/>
     </row>
-    <row r="298" spans="1:9" ht="15.6">
+    <row r="298" spans="1:9" ht="15.75">
       <c r="A298" s="17" t="b">
         <v>0</v>
       </c>
@@ -17455,7 +17455,7 @@
       <c r="H298" s="17"/>
       <c r="I298" s="17"/>
     </row>
-    <row r="299" spans="1:9" ht="15.6">
+    <row r="299" spans="1:9" ht="15.75">
       <c r="A299" s="17"/>
       <c r="B299" s="17" t="s">
         <v>21</v>
@@ -17480,7 +17480,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.6">
+    <row r="300" spans="1:9" ht="15.75">
       <c r="A300" s="17"/>
       <c r="B300" s="17" t="s">
         <v>21</v>
@@ -17503,7 +17503,7 @@
       </c>
       <c r="I300" s="17"/>
     </row>
-    <row r="301" spans="1:9" ht="15.6">
+    <row r="301" spans="1:9" ht="15.75">
       <c r="A301" s="17"/>
       <c r="B301" s="17" t="s">
         <v>21</v>
@@ -17526,7 +17526,7 @@
       </c>
       <c r="I301" s="17"/>
     </row>
-    <row r="302" spans="1:9" ht="15.6">
+    <row r="302" spans="1:9" ht="15.75">
       <c r="A302" s="17"/>
       <c r="B302" s="17" t="s">
         <v>21</v>
@@ -17549,7 +17549,7 @@
       </c>
       <c r="I302" s="17"/>
     </row>
-    <row r="303" spans="1:9" ht="15.6">
+    <row r="303" spans="1:9" ht="15.75">
       <c r="A303" s="17"/>
       <c r="B303" s="17" t="s">
         <v>21</v>
@@ -17572,7 +17572,7 @@
       </c>
       <c r="I303" s="17"/>
     </row>
-    <row r="304" spans="1:9" ht="15.6">
+    <row r="304" spans="1:9" ht="15.75">
       <c r="A304" s="17"/>
       <c r="B304" s="17" t="s">
         <v>21</v>
@@ -17595,7 +17595,7 @@
       </c>
       <c r="I304" s="17"/>
     </row>
-    <row r="305" spans="1:9" ht="15.6">
+    <row r="305" spans="1:9" ht="15.75">
       <c r="A305" s="17"/>
       <c r="B305" s="17" t="s">
         <v>21</v>
@@ -17618,7 +17618,7 @@
       </c>
       <c r="I305" s="17"/>
     </row>
-    <row r="306" spans="1:9" ht="15.6">
+    <row r="306" spans="1:9" ht="15.75">
       <c r="A306" s="17"/>
       <c r="B306" s="17" t="s">
         <v>21</v>
@@ -17641,7 +17641,7 @@
       </c>
       <c r="I306" s="17"/>
     </row>
-    <row r="307" spans="1:9" ht="15.6">
+    <row r="307" spans="1:9" ht="15.75">
       <c r="A307" s="17"/>
       <c r="B307" s="17" t="s">
         <v>21</v>
@@ -17664,7 +17664,7 @@
       </c>
       <c r="I307" s="17"/>
     </row>
-    <row r="308" spans="1:9" ht="15.6">
+    <row r="308" spans="1:9" ht="15.75">
       <c r="A308" s="17" t="b">
         <v>0</v>
       </c>
@@ -17683,7 +17683,7 @@
       <c r="H308" s="17"/>
       <c r="I308" s="17"/>
     </row>
-    <row r="309" spans="1:9" ht="15.6">
+    <row r="309" spans="1:9" ht="15.75">
       <c r="A309" s="17"/>
       <c r="B309" s="17" t="s">
         <v>21</v>
@@ -17706,7 +17706,7 @@
       </c>
       <c r="I309" s="17"/>
     </row>
-    <row r="310" spans="1:9" ht="15.6">
+    <row r="310" spans="1:9" ht="15.75">
       <c r="A310" s="17"/>
       <c r="B310" s="17" t="s">
         <v>21</v>
@@ -17729,7 +17729,7 @@
       </c>
       <c r="I310" s="17"/>
     </row>
-    <row r="311" spans="1:9" ht="15.6">
+    <row r="311" spans="1:9" ht="15.75">
       <c r="A311" s="17"/>
       <c r="B311" s="17" t="s">
         <v>21</v>
@@ -17752,7 +17752,7 @@
       </c>
       <c r="I311" s="17"/>
     </row>
-    <row r="312" spans="1:9" ht="15.6">
+    <row r="312" spans="1:9" ht="15.75">
       <c r="A312" s="17"/>
       <c r="B312" s="17" t="s">
         <v>21</v>
@@ -17775,7 +17775,7 @@
       </c>
       <c r="I312" s="17"/>
     </row>
-    <row r="313" spans="1:9" ht="15.6">
+    <row r="313" spans="1:9" ht="15.75">
       <c r="A313" s="17" t="b">
         <v>0</v>
       </c>
@@ -17794,7 +17794,7 @@
       <c r="H313" s="17"/>
       <c r="I313" s="17"/>
     </row>
-    <row r="314" spans="1:9" ht="15.6">
+    <row r="314" spans="1:9" ht="15.75">
       <c r="A314" s="17"/>
       <c r="B314" s="17" t="s">
         <v>21</v>
@@ -17817,7 +17817,7 @@
       </c>
       <c r="I314" s="17"/>
     </row>
-    <row r="315" spans="1:9" ht="15.6">
+    <row r="315" spans="1:9" ht="15.75">
       <c r="A315" s="17"/>
       <c r="B315" s="17" t="s">
         <v>21</v>
@@ -17840,7 +17840,7 @@
       </c>
       <c r="I315" s="17"/>
     </row>
-    <row r="316" spans="1:9" ht="15.6">
+    <row r="316" spans="1:9" ht="15.75">
       <c r="A316" s="17"/>
       <c r="B316" s="17" t="s">
         <v>21</v>
@@ -17865,7 +17865,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.6">
+    <row r="317" spans="1:9" ht="15.75">
       <c r="A317" s="17" t="b">
         <v>0</v>
       </c>
@@ -17884,7 +17884,7 @@
       <c r="H317" s="17"/>
       <c r="I317" s="17"/>
     </row>
-    <row r="318" spans="1:9" ht="15.6">
+    <row r="318" spans="1:9" ht="15.75">
       <c r="A318" s="17"/>
       <c r="B318" s="17" t="s">
         <v>21</v>
@@ -17909,7 +17909,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.6">
+    <row r="319" spans="1:9" ht="15.75">
       <c r="A319" s="17"/>
       <c r="B319" s="17" t="s">
         <v>21</v>
@@ -17932,7 +17932,7 @@
       </c>
       <c r="I319" s="17"/>
     </row>
-    <row r="320" spans="1:9" ht="15.6">
+    <row r="320" spans="1:9" ht="15.75">
       <c r="A320" s="17" t="b">
         <v>0</v>
       </c>
@@ -17951,7 +17951,7 @@
       <c r="H320" s="17"/>
       <c r="I320" s="17"/>
     </row>
-    <row r="321" spans="1:9" ht="15.6">
+    <row r="321" spans="1:9" ht="15.75">
       <c r="A321" s="17"/>
       <c r="B321" s="17" t="s">
         <v>21</v>
@@ -17972,7 +17972,7 @@
       <c r="H321" s="17"/>
       <c r="I321" s="17"/>
     </row>
-    <row r="322" spans="1:9" ht="15.6">
+    <row r="322" spans="1:9" ht="15.75">
       <c r="A322" s="17"/>
       <c r="B322" s="17" t="s">
         <v>21</v>
@@ -17993,7 +17993,7 @@
       <c r="H322" s="17"/>
       <c r="I322" s="17"/>
     </row>
-    <row r="323" spans="1:9" ht="15.6">
+    <row r="323" spans="1:9" ht="15.75">
       <c r="A323" s="17"/>
       <c r="B323" s="17" t="s">
         <v>21</v>
@@ -18016,7 +18016,7 @@
       </c>
       <c r="I323" s="17"/>
     </row>
-    <row r="324" spans="1:9" ht="15.6">
+    <row r="324" spans="1:9" ht="15.75">
       <c r="A324" s="17" t="b">
         <v>0</v>
       </c>
@@ -18035,7 +18035,7 @@
       <c r="H324" s="17"/>
       <c r="I324" s="17"/>
     </row>
-    <row r="325" spans="1:9" ht="15.6">
+    <row r="325" spans="1:9" ht="15.75">
       <c r="A325" s="17" t="b">
         <v>0</v>
       </c>
@@ -18054,7 +18054,7 @@
       <c r="H325" s="17"/>
       <c r="I325" s="17"/>
     </row>
-    <row r="326" spans="1:9" ht="15.6">
+    <row r="326" spans="1:9" ht="15.75">
       <c r="A326" s="17"/>
       <c r="B326" s="17" t="s">
         <v>21</v>
@@ -18079,7 +18079,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.6">
+    <row r="327" spans="1:9" ht="15.75">
       <c r="A327" s="17"/>
       <c r="B327" s="17" t="s">
         <v>21</v>
@@ -18436,7 +18436,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15.6">
+    <row r="344" spans="1:16" ht="15.75">
       <c r="A344" s="17"/>
       <c r="B344" t="s">
         <v>21</v>
@@ -18799,7 +18799,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.6">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.75">
       <c r="A362" s="17"/>
       <c r="B362" t="s">
         <v>22</v>
@@ -18927,14 +18927,14 @@
       <selection activeCell="O17" sqref="O17:Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
-    <col min="17" max="17" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="17" max="17" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -19387,13 +19387,13 @@
         <v>574</v>
       </c>
       <c r="O25" s="31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="P25" s="30">
         <v>1</v>
       </c>
       <c r="Q25" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="26" spans="1:17">

</xml_diff>

<commit_message>
Cleaning up amy files, can't get it to run
Just dropped in epw, but not stat and ddy.
</commit_message>
<xml_diff>
--- a/projects/office_calibration_nsga2_14.xlsx
+++ b/projects/office_calibration_nsga2_14.xlsx
@@ -2476,7 +2476,7 @@
     <t>2013-12-12</t>
   </si>
   <si>
-    <t>SPtMasterTable_15084_2013_amy.epw</t>
+    <t>USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
   </si>
 </sst>
 </file>
@@ -6769,7 +6769,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -7028,7 +7028,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="30">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>579</v>
@@ -7040,7 +7040,7 @@
         <v>564</v>
       </c>
       <c r="B25" s="30">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>578</v>
@@ -7250,9 +7250,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated to use AMY what is running now
changes to spreadsheet, and renamed copy of logan stat and ddy
</commit_message>
<xml_diff>
--- a/projects/office_calibration_nsga2_14.xlsx
+++ b/projects/office_calibration_nsga2_14.xlsx
@@ -2476,7 +2476,7 @@
     <t>2013-12-12</t>
   </si>
   <si>
-    <t>USA_MA_Boston-Logan.Intl.AP.725090_TMY3.epw</t>
+    <t>SPtMasterTable_15084_2013_amy.epw</t>
   </si>
 </sst>
 </file>
@@ -6768,7 +6768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -7252,7 +7252,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Adding SWH measure to all spreadsheets
It is in model 0 but also used as calibration.
</commit_message>
<xml_diff>
--- a/projects/office_calibration_nsga2_14.xlsx
+++ b/projects/office_calibration_nsga2_14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="13170" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$Z$154</definedName>
     <definedName name="AnalysisType">Lookups!$A$17:$A$23</definedName>
     <definedName name="instance_defs">Lookups!$A$2:$D$9</definedName>
     <definedName name="instance_types">Lookups!$A$2:$A$9</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="820">
   <si>
     <t>type</t>
   </si>
@@ -2477,6 +2477,30 @@
   </si>
   <si>
     <t>SPtMasterTable_15084_2013_amy.epw</t>
+  </si>
+  <si>
+    <t>Add Service Water Heating</t>
+  </si>
+  <si>
+    <t>AddServiceWaterHeating</t>
+  </si>
+  <si>
+    <t>Water Heater Fuel Type</t>
+  </si>
+  <si>
+    <t>water_heater_fuel_type</t>
+  </si>
+  <si>
+    <t>NaturalGas</t>
+  </si>
+  <si>
+    <t>Gallons Hot Water per Occupant per Day</t>
+  </si>
+  <si>
+    <t>hot_water_per_occ_per_day_gal</t>
+  </si>
+  <si>
+    <t>gal</t>
   </si>
 </sst>
 </file>
@@ -6768,7 +6792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -7248,11 +7272,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y224"/>
+  <dimension ref="A1:Y227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8642,161 +8666,165 @@
         <v>1</v>
       </c>
       <c r="B59" s="38" t="s">
-        <v>704</v>
+        <v>812</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>703</v>
+        <v>813</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>703</v>
+        <v>813</v>
       </c>
       <c r="E59" s="38" t="s">
-        <v>233</v>
+        <v>68</v>
       </c>
       <c r="G59" s="39"/>
       <c r="H59" s="39"/>
     </row>
-    <row r="60" spans="1:17" s="49" customFormat="1">
-      <c r="A60" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B60" s="49" t="s">
-        <v>751</v>
-      </c>
-      <c r="C60" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="49" t="s">
-        <v>68</v>
-      </c>
+    <row r="60" spans="1:17">
+      <c r="B60" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>814</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>815</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>816</v>
+      </c>
+      <c r="I60" s="31"/>
     </row>
     <row r="61" spans="1:17" s="43" customFormat="1">
       <c r="B61" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>752</v>
+        <v>817</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>77</v>
+        <v>818</v>
       </c>
       <c r="F61" s="43" t="s">
-        <v>64</v>
+        <v>619</v>
+      </c>
+      <c r="G61" s="43" t="s">
+        <v>819</v>
       </c>
       <c r="H61" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="J61" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="K61" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="L61" s="43">
-        <v>0.4</v>
+        <v>1</v>
+      </c>
+      <c r="J61" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="K61" s="45">
+        <v>3</v>
+      </c>
+      <c r="L61" s="45">
+        <v>1</v>
       </c>
       <c r="M61" s="43">
-        <f>(K61+J61)/6</f>
-        <v>0.14166666666666669</v>
+        <f>(K61-J61)/6</f>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N61" s="43">
-        <v>0.1</v>
-      </c>
+        <v>0.01</v>
+      </c>
+      <c r="P61" s="47"/>
       <c r="Q61" s="43" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="62" spans="1:17" s="30" customFormat="1">
-      <c r="B62" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D62" s="30" t="s">
+    <row r="62" spans="1:17" s="38" customFormat="1">
+      <c r="A62" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>704</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>703</v>
+      </c>
+      <c r="D62" s="38" t="s">
+        <v>703</v>
+      </c>
+      <c r="E62" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+    </row>
+    <row r="63" spans="1:17" s="49" customFormat="1">
+      <c r="A63" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>751</v>
+      </c>
+      <c r="C63" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E63" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="43" customFormat="1">
+      <c r="B64" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" s="43" t="s">
+        <v>752</v>
+      </c>
+      <c r="E64" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="J64" s="43">
+        <v>0.05</v>
+      </c>
+      <c r="K64" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="L64" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="M64" s="43">
+        <f>(K64+J64)/6</f>
+        <v>0.14166666666666669</v>
+      </c>
+      <c r="N64" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="Q64" s="43" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="30" customFormat="1">
+      <c r="B65" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E65" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F62" s="30" t="s">
+      <c r="F65" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H62" s="30">
+      <c r="H65" s="30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" s="30" customFormat="1">
-      <c r="B63" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D63" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F63" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H63" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="I63" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" s="49" customFormat="1">
-      <c r="A64" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B64" s="49" t="s">
-        <v>754</v>
-      </c>
-      <c r="C64" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="E64" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" s="43" customFormat="1">
-      <c r="B65" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D65" s="43" t="s">
-        <v>755</v>
-      </c>
-      <c r="E65" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="F65" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H65" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="J65" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="K65" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="L65" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="M65" s="43">
-        <f>(K65+J65)/6</f>
-        <v>0.14166666666666669</v>
-      </c>
-      <c r="N65" s="43">
-        <v>0.1</v>
-      </c>
-      <c r="Q65" s="43" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="66" spans="1:17" s="30" customFormat="1">
@@ -8804,89 +8832,89 @@
         <v>21</v>
       </c>
       <c r="D66" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I66" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" s="49" customFormat="1">
+      <c r="A67" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B67" s="49" t="s">
+        <v>754</v>
+      </c>
+      <c r="C67" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" s="43" customFormat="1">
+      <c r="B68" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>755</v>
+      </c>
+      <c r="E68" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F68" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="J68" s="43">
+        <v>0.05</v>
+      </c>
+      <c r="K68" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="L68" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="M68" s="43">
+        <f>(K68+J68)/6</f>
+        <v>0.14166666666666669</v>
+      </c>
+      <c r="N68" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="Q68" s="43" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" s="30" customFormat="1">
+      <c r="B69" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="E66" s="30" t="s">
+      <c r="E69" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="F66" s="30" t="s">
+      <c r="F69" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H66" s="30">
+      <c r="H69" s="30">
         <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" s="30" customFormat="1">
-      <c r="B67" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E67" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F67" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H67" s="30" t="s">
-        <v>669</v>
-      </c>
-      <c r="I67" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" s="49" customFormat="1">
-      <c r="A68" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B68" s="49" t="s">
-        <v>756</v>
-      </c>
-      <c r="C68" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D68" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="E68" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" s="43" customFormat="1">
-      <c r="B69" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D69" s="43" t="s">
-        <v>757</v>
-      </c>
-      <c r="E69" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="F69" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H69" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="J69" s="43">
-        <v>0.05</v>
-      </c>
-      <c r="K69" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="L69" s="43">
-        <v>0.4</v>
-      </c>
-      <c r="M69" s="43">
-        <f>(K69+J69)/6</f>
-        <v>0.14166666666666669</v>
-      </c>
-      <c r="N69" s="43">
-        <v>0.1</v>
-      </c>
-      <c r="Q69" s="43" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="30" customFormat="1">
@@ -8894,53 +8922,72 @@
         <v>21</v>
       </c>
       <c r="D70" s="30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F70" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H70" s="30" t="s">
+        <v>669</v>
+      </c>
+      <c r="I70" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" s="49" customFormat="1">
+      <c r="A71" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71" s="49" t="s">
+        <v>756</v>
+      </c>
+      <c r="C71" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" s="49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="43" customFormat="1">
+      <c r="B72" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>757</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F72" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H70" s="30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" s="30" customFormat="1">
-      <c r="B71" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E71" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F71" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H71" s="30" t="s">
-        <v>670</v>
-      </c>
-      <c r="I71" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" s="49" customFormat="1">
-      <c r="A72" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B72" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="E72" s="49" t="s">
-        <v>68</v>
+      <c r="H72" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="J72" s="43">
+        <v>0.05</v>
+      </c>
+      <c r="K72" s="43">
+        <v>0.8</v>
+      </c>
+      <c r="L72" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="M72" s="43">
+        <f>(K72+J72)/6</f>
+        <v>0.14166666666666669</v>
+      </c>
+      <c r="N72" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="Q72" s="43" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="30" customFormat="1">
@@ -8948,221 +8995,182 @@
         <v>21</v>
       </c>
       <c r="D73" s="30" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F73" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" s="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="30" customFormat="1">
+      <c r="B74" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F74" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H73" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I73" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="O73" s="31"/>
-    </row>
-    <row r="74" spans="1:17" s="43" customFormat="1">
-      <c r="B74" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D74" s="44" t="s">
-        <v>758</v>
-      </c>
-      <c r="E74" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F74" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H74" s="43">
-        <v>0</v>
-      </c>
-      <c r="J74" s="45">
-        <v>-100</v>
-      </c>
-      <c r="K74" s="45">
-        <v>100</v>
-      </c>
-      <c r="L74" s="45">
-        <v>0</v>
-      </c>
-      <c r="M74" s="45">
-        <f>(K74-J74)/6</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="N74" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q74" s="43" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" s="30" customFormat="1">
-      <c r="B75" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E75" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F75" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="H75" s="30">
-        <v>0</v>
-      </c>
-      <c r="O75" s="31"/>
+      <c r="H74" s="30" t="s">
+        <v>670</v>
+      </c>
+      <c r="I74" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="49" customFormat="1">
+      <c r="A75" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B75" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="49" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="76" spans="1:17" s="30" customFormat="1">
       <c r="B76" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D76" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H76" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I76" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="O76" s="31"/>
+    </row>
+    <row r="77" spans="1:17" s="43" customFormat="1">
+      <c r="B77" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D77" s="44" t="s">
+        <v>758</v>
+      </c>
+      <c r="E77" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F77" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H77" s="43">
+        <v>0</v>
+      </c>
+      <c r="J77" s="45">
+        <v>-100</v>
+      </c>
+      <c r="K77" s="45">
+        <v>100</v>
+      </c>
+      <c r="L77" s="45">
+        <v>0</v>
+      </c>
+      <c r="M77" s="45">
+        <f>(K77-J77)/6</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="N77" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q77" s="43" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="30" customFormat="1">
+      <c r="B78" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H78" s="30">
+        <v>0</v>
+      </c>
+      <c r="O78" s="31"/>
+    </row>
+    <row r="79" spans="1:17" s="30" customFormat="1">
+      <c r="B79" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E79" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F76" s="30" t="s">
+      <c r="F79" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H76" s="30">
-        <v>0</v>
-      </c>
-      <c r="O76" s="31"/>
-    </row>
-    <row r="77" spans="1:17" s="30" customFormat="1">
-      <c r="B77" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D77" s="30" t="s">
+      <c r="H79" s="30">
+        <v>0</v>
+      </c>
+      <c r="O79" s="31"/>
+    </row>
+    <row r="80" spans="1:17" s="30" customFormat="1">
+      <c r="B80" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E80" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F77" s="30" t="s">
+      <c r="F80" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H77" s="30">
+      <c r="H80" s="30">
         <v>1</v>
       </c>
-      <c r="O77" s="31"/>
-    </row>
-    <row r="78" spans="1:17" s="50" customFormat="1">
-      <c r="A78" s="50" t="b">
+      <c r="O80" s="31"/>
+    </row>
+    <row r="81" spans="1:17" s="50" customFormat="1">
+      <c r="A81" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B78" s="50" t="s">
+      <c r="B81" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C78" s="50" t="s">
+      <c r="C81" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D78" s="50" t="s">
+      <c r="D81" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="E78" s="50" t="s">
+      <c r="E81" s="50" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="79" spans="1:17">
-      <c r="A79" s="30"/>
-      <c r="B79" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F79" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G79" s="30"/>
-      <c r="H79" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I79" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
-      <c r="P79" s="40"/>
-    </row>
-    <row r="80" spans="1:17" s="43" customFormat="1">
-      <c r="B80" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D80" s="43" t="s">
-        <v>759</v>
-      </c>
-      <c r="E80" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F80" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H80" s="43">
-        <v>0</v>
-      </c>
-      <c r="I80" s="46"/>
-      <c r="J80" s="45">
-        <v>-60</v>
-      </c>
-      <c r="K80" s="45">
-        <v>60</v>
-      </c>
-      <c r="L80" s="45">
-        <v>-1</v>
-      </c>
-      <c r="M80" s="45">
-        <f>(K80-J80)/6</f>
-        <v>20</v>
-      </c>
-      <c r="N80" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="P80" s="47"/>
-      <c r="Q80" s="43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F81" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G81" s="30"/>
-      <c r="H81" s="30">
-        <v>0</v>
-      </c>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
-      <c r="P81" s="40"/>
     </row>
     <row r="82" spans="1:17">
       <c r="A82" s="30"/>
@@ -9171,17 +9179,20 @@
       </c>
       <c r="C82" s="30"/>
       <c r="D82" s="30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F82" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G82" s="30"/>
-      <c r="H82" s="30">
-        <v>0</v>
+      <c r="H82" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I82" s="30" t="s">
+        <v>83</v>
       </c>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -9190,31 +9201,43 @@
       <c r="N82" s="3"/>
       <c r="P82" s="40"/>
     </row>
-    <row r="83" spans="1:17">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F83" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G83" s="30"/>
-      <c r="H83" s="30">
-        <v>0</v>
-      </c>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="P83" s="40"/>
+    <row r="83" spans="1:17" s="43" customFormat="1">
+      <c r="B83" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D83" s="43" t="s">
+        <v>759</v>
+      </c>
+      <c r="E83" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F83" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H83" s="43">
+        <v>0</v>
+      </c>
+      <c r="I83" s="46"/>
+      <c r="J83" s="45">
+        <v>-60</v>
+      </c>
+      <c r="K83" s="45">
+        <v>60</v>
+      </c>
+      <c r="L83" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M83" s="45">
+        <f>(K83-J83)/6</f>
+        <v>20</v>
+      </c>
+      <c r="N83" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="P83" s="47"/>
+      <c r="Q83" s="43" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="84" spans="1:17">
       <c r="A84" s="30"/>
@@ -9222,18 +9245,18 @@
         <v>21</v>
       </c>
       <c r="C84" s="30"/>
-      <c r="D84" s="30" t="s">
-        <v>53</v>
+      <c r="D84" s="48" t="s">
+        <v>47</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F84" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G84" s="30"/>
-      <c r="H84" s="30" t="b">
-        <v>1</v>
+      <c r="H84" s="30">
+        <v>0</v>
       </c>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -9249,17 +9272,17 @@
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F85" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G85" s="30"/>
       <c r="H85" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -9275,13 +9298,13 @@
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F86" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G86" s="30"/>
       <c r="H86" s="30">
@@ -9301,16 +9324,16 @@
       </c>
       <c r="C87" s="30"/>
       <c r="D87" s="30" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F87" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G87" s="30"/>
-      <c r="H87" s="30">
+      <c r="H87" s="30" t="b">
         <v>1</v>
       </c>
       <c r="J87" s="3"/>
@@ -9320,22 +9343,31 @@
       <c r="N87" s="3"/>
       <c r="P87" s="40"/>
     </row>
-    <row r="88" spans="1:17" s="50" customFormat="1">
-      <c r="A88" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B88" s="50" t="s">
-        <v>327</v>
-      </c>
-      <c r="C88" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="D88" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="E88" s="50" t="s">
-        <v>68</v>
-      </c>
+    <row r="88" spans="1:17">
+      <c r="A88" s="30"/>
+      <c r="B88" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F88" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G88" s="30"/>
+      <c r="H88" s="30">
+        <v>15</v>
+      </c>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="P88" s="40"/>
     </row>
     <row r="89" spans="1:17">
       <c r="A89" s="30"/>
@@ -9344,20 +9376,17 @@
       </c>
       <c r="C89" s="30"/>
       <c r="D89" s="30" t="s">
-        <v>373</v>
+        <v>57</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F89" s="30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G89" s="30"/>
-      <c r="H89" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I89" s="30" t="s">
-        <v>83</v>
+      <c r="H89" s="30">
+        <v>0</v>
       </c>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
@@ -9366,186 +9395,184 @@
       <c r="N89" s="3"/>
       <c r="P89" s="40"/>
     </row>
-    <row r="90" spans="1:17" s="43" customFormat="1">
-      <c r="B90" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D90" s="43" t="s">
-        <v>777</v>
-      </c>
-      <c r="E90" s="43" t="s">
-        <v>330</v>
-      </c>
-      <c r="F90" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H90" s="43">
-        <v>0</v>
-      </c>
-      <c r="I90" s="46"/>
-      <c r="J90" s="45">
-        <v>-30</v>
-      </c>
-      <c r="K90" s="45">
-        <v>30</v>
-      </c>
-      <c r="L90" s="45">
-        <v>0</v>
-      </c>
-      <c r="M90" s="45">
-        <f>(K90-J90)/6</f>
-        <v>10</v>
-      </c>
-      <c r="N90" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q90" s="43" t="s">
-        <v>753</v>
-      </c>
+    <row r="90" spans="1:17">
+      <c r="A90" s="30"/>
+      <c r="B90" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E90" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F90" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G90" s="30"/>
+      <c r="H90" s="30">
+        <v>1</v>
+      </c>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="P90" s="40"/>
     </row>
     <row r="91" spans="1:17" s="50" customFormat="1">
       <c r="A91" s="50" t="b">
         <v>1</v>
       </c>
       <c r="B91" s="50" t="s">
-        <v>778</v>
+        <v>327</v>
       </c>
       <c r="C91" s="50" t="s">
-        <v>779</v>
+        <v>328</v>
       </c>
       <c r="D91" s="50" t="s">
-        <v>779</v>
+        <v>328</v>
       </c>
       <c r="E91" s="50" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="43" customFormat="1">
-      <c r="B92" s="43" t="s">
+    <row r="92" spans="1:17">
+      <c r="A92" s="30"/>
+      <c r="B92" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E92" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F92" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="G92" s="30"/>
+      <c r="H92" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I92" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="P92" s="40"/>
+    </row>
+    <row r="93" spans="1:17" s="43" customFormat="1">
+      <c r="B93" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D92" s="43" t="s">
+      <c r="D93" s="43" t="s">
+        <v>777</v>
+      </c>
+      <c r="E93" s="43" t="s">
+        <v>330</v>
+      </c>
+      <c r="F93" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H93" s="43">
+        <v>0</v>
+      </c>
+      <c r="I93" s="46"/>
+      <c r="J93" s="45">
+        <v>-30</v>
+      </c>
+      <c r="K93" s="45">
+        <v>30</v>
+      </c>
+      <c r="L93" s="45">
+        <v>0</v>
+      </c>
+      <c r="M93" s="45">
+        <f>(K93-J93)/6</f>
+        <v>10</v>
+      </c>
+      <c r="N93" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q93" s="43" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="50" customFormat="1">
+      <c r="A94" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B94" s="50" t="s">
+        <v>778</v>
+      </c>
+      <c r="C94" s="50" t="s">
+        <v>779</v>
+      </c>
+      <c r="D94" s="50" t="s">
+        <v>779</v>
+      </c>
+      <c r="E94" s="50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" s="43" customFormat="1">
+      <c r="B95" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" s="43" t="s">
         <v>780</v>
       </c>
-      <c r="E92" s="43" t="s">
+      <c r="E95" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="F92" s="43" t="s">
+      <c r="F95" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H92" s="43">
-        <v>0</v>
-      </c>
-      <c r="I92" s="46"/>
-      <c r="J92" s="45">
+      <c r="H95" s="43">
+        <v>0</v>
+      </c>
+      <c r="I95" s="46"/>
+      <c r="J95" s="45">
         <v>-50</v>
       </c>
-      <c r="K92" s="45">
+      <c r="K95" s="45">
         <v>100</v>
       </c>
-      <c r="L92" s="45">
-        <v>0</v>
-      </c>
-      <c r="M92" s="45">
-        <f>(K92-J92)/6</f>
+      <c r="L95" s="45">
+        <v>0</v>
+      </c>
+      <c r="M95" s="45">
+        <f>(K95-J95)/6</f>
         <v>25</v>
       </c>
-      <c r="N92" s="45">
+      <c r="N95" s="45">
         <v>2.5</v>
       </c>
-      <c r="Q92" s="43" t="s">
+      <c r="Q95" s="43" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="50" customFormat="1">
-      <c r="A93" s="50" t="b">
+    <row r="96" spans="1:17" s="50" customFormat="1">
+      <c r="A96" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="B93" s="50" t="s">
+      <c r="B96" s="50" t="s">
         <v>781</v>
       </c>
-      <c r="C93" s="50" t="s">
+      <c r="C96" s="50" t="s">
         <v>782</v>
       </c>
-      <c r="D93" s="50" t="s">
+      <c r="D96" s="50" t="s">
         <v>782</v>
       </c>
-      <c r="E93" s="50" t="s">
+      <c r="E96" s="50" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" s="43" customFormat="1">
-      <c r="B94" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D94" s="43" t="s">
-        <v>783</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>258</v>
-      </c>
-      <c r="F94" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="H94" s="43">
-        <v>0</v>
-      </c>
-      <c r="I94" s="46"/>
-      <c r="J94" s="45">
-        <v>-50</v>
-      </c>
-      <c r="K94" s="45">
-        <v>100</v>
-      </c>
-      <c r="L94" s="45">
-        <v>0</v>
-      </c>
-      <c r="M94" s="45">
-        <f>(K94-J94)/6</f>
-        <v>25</v>
-      </c>
-      <c r="N94" s="45">
-        <v>2.5</v>
-      </c>
-      <c r="Q94" s="43" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" s="50" customFormat="1">
-      <c r="A95" s="50" t="b">
-        <v>1</v>
-      </c>
-      <c r="B95" s="50" t="s">
-        <v>285</v>
-      </c>
-      <c r="C95" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="D95" s="50" t="s">
-        <v>286</v>
-      </c>
-      <c r="E95" s="50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" s="30" customFormat="1">
-      <c r="B96" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F96" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H96" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I96" s="30" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:17" s="43" customFormat="1">
@@ -9553,33 +9580,30 @@
         <v>22</v>
       </c>
       <c r="D97" s="43" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>288</v>
+        <v>258</v>
       </c>
       <c r="F97" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G97" s="43" t="s">
-        <v>785</v>
-      </c>
       <c r="H97" s="43">
         <v>0</v>
       </c>
       <c r="I97" s="46"/>
       <c r="J97" s="45">
-        <v>-40</v>
+        <v>-50</v>
       </c>
       <c r="K97" s="45">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="L97" s="45">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M97" s="45">
         <f>(K97-J97)/6</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N97" s="45">
         <v>2.5</v>
@@ -9588,24 +9612,21 @@
         <v>753</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="30" customFormat="1">
-      <c r="B98" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>786</v>
-      </c>
-      <c r="E98" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F98" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="G98" s="30" t="s">
-        <v>785</v>
-      </c>
-      <c r="H98" s="30">
-        <v>0</v>
+    <row r="98" spans="1:17" s="50" customFormat="1">
+      <c r="A98" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="B98" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="C98" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="E98" s="50" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:17" s="30" customFormat="1">
@@ -9613,39 +9634,59 @@
         <v>21</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>787</v>
+        <v>373</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F99" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H99" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I99" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" s="43" customFormat="1">
+      <c r="B100" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D100" s="43" t="s">
+        <v>784</v>
+      </c>
+      <c r="E100" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="F100" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G99" s="30" t="s">
+      <c r="G100" s="43" t="s">
         <v>785</v>
       </c>
-      <c r="H99" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" s="30" customFormat="1">
-      <c r="B100" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D100" s="30" t="s">
-        <v>788</v>
-      </c>
-      <c r="E100" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F100" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G100" s="30" t="s">
-        <v>789</v>
-      </c>
-      <c r="H100" s="30">
-        <v>0</v>
+      <c r="H100" s="43">
+        <v>0</v>
+      </c>
+      <c r="I100" s="46"/>
+      <c r="J100" s="45">
+        <v>-40</v>
+      </c>
+      <c r="K100" s="45">
+        <v>80</v>
+      </c>
+      <c r="L100" s="45">
+        <v>-1</v>
+      </c>
+      <c r="M100" s="45">
+        <f>(K100-J100)/6</f>
+        <v>20</v>
+      </c>
+      <c r="N100" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="Q100" s="43" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="101" spans="1:17" s="30" customFormat="1">
@@ -9653,15 +9694,18 @@
         <v>21</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F101" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H101" s="30" t="b">
+        <v>64</v>
+      </c>
+      <c r="G101" s="30" t="s">
+        <v>785</v>
+      </c>
+      <c r="H101" s="30">
         <v>0</v>
       </c>
     </row>
@@ -9670,19 +9714,19 @@
         <v>21</v>
       </c>
       <c r="D102" s="30" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F102" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G102" s="30" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="H102" s="30">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="30" customFormat="1">
@@ -9690,16 +9734,16 @@
         <v>21</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F103" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G103" s="30" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="H103" s="30">
         <v>0</v>
@@ -9710,153 +9754,198 @@
         <v>21</v>
       </c>
       <c r="D104" s="30" t="s">
+        <v>790</v>
+      </c>
+      <c r="E104" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H104" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" s="30" customFormat="1">
+      <c r="B105" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>791</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F105" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="G105" s="30" t="s">
+        <v>789</v>
+      </c>
+      <c r="H105" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" s="30" customFormat="1">
+      <c r="B106" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>792</v>
+      </c>
+      <c r="E106" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G106" s="30" t="s">
+        <v>785</v>
+      </c>
+      <c r="H106" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" s="30" customFormat="1">
+      <c r="B107" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="30" t="s">
         <v>793</v>
       </c>
-      <c r="E104" s="30" t="s">
+      <c r="E107" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F104" s="30" t="s">
+      <c r="F107" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G104" s="30" t="s">
+      <c r="G107" s="30" t="s">
         <v>789</v>
       </c>
-      <c r="H104" s="30">
+      <c r="H107" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:17" s="38" customFormat="1">
-      <c r="A105" s="38" t="b">
+    <row r="108" spans="1:17" s="38" customFormat="1">
+      <c r="A108" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="B105" s="38" t="s">
+      <c r="B108" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="C105" s="38" t="s">
+      <c r="C108" s="38" t="s">
         <v>802</v>
       </c>
-      <c r="D105" s="38" t="s">
+      <c r="D108" s="38" t="s">
         <v>802</v>
       </c>
-      <c r="E105" s="38" t="s">
+      <c r="E108" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="G105" s="39"/>
-      <c r="H105" s="39"/>
-    </row>
-    <row r="106" spans="1:17" s="43" customFormat="1">
-      <c r="B106" s="43" t="s">
+      <c r="G108" s="39"/>
+      <c r="H108" s="39"/>
+    </row>
+    <row r="109" spans="1:17" s="43" customFormat="1">
+      <c r="B109" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D106" s="43" t="s">
+      <c r="D109" s="43" t="s">
         <v>803</v>
       </c>
-      <c r="E106" s="43" t="s">
+      <c r="E109" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F106" s="43" t="s">
+      <c r="F109" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G106" s="43" t="s">
+      <c r="G109" s="43" t="s">
         <v>804</v>
       </c>
-      <c r="H106" s="43">
+      <c r="H109" s="43">
         <v>1</v>
       </c>
-      <c r="I106" s="46"/>
-      <c r="J106" s="45">
+      <c r="I109" s="46"/>
+      <c r="J109" s="45">
         <v>-2</v>
       </c>
-      <c r="K106" s="45">
-        <v>2</v>
-      </c>
-      <c r="L106" s="45">
-        <v>0</v>
-      </c>
-      <c r="M106" s="45">
-        <f>(K106-J106)/6</f>
+      <c r="K109" s="45">
+        <v>2</v>
+      </c>
+      <c r="L109" s="45">
+        <v>0</v>
+      </c>
+      <c r="M109" s="45">
+        <f>(K109-J109)/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N106" s="45">
+      <c r="N109" s="45">
         <v>1</v>
       </c>
-      <c r="Q106" s="43" t="s">
+      <c r="Q109" s="43" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="107" spans="1:17" s="43" customFormat="1">
-      <c r="B107" s="43" t="s">
+    <row r="110" spans="1:17" s="43" customFormat="1">
+      <c r="B110" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D107" s="43" t="s">
+      <c r="D110" s="43" t="s">
         <v>805</v>
       </c>
-      <c r="E107" s="43" t="s">
+      <c r="E110" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="F107" s="43" t="s">
+      <c r="F110" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G107" s="43" t="s">
+      <c r="G110" s="43" t="s">
         <v>804</v>
       </c>
-      <c r="H107" s="43">
+      <c r="H110" s="43">
         <v>-1</v>
       </c>
-      <c r="I107" s="46"/>
-      <c r="J107" s="45">
+      <c r="I110" s="46"/>
+      <c r="J110" s="45">
         <v>-2</v>
       </c>
-      <c r="K107" s="45">
-        <v>2</v>
-      </c>
-      <c r="L107" s="45">
-        <v>0</v>
-      </c>
-      <c r="M107" s="45">
-        <f>(K107-J107)/6</f>
+      <c r="K110" s="45">
+        <v>2</v>
+      </c>
+      <c r="L110" s="45">
+        <v>0</v>
+      </c>
+      <c r="M110" s="45">
+        <f>(K110-J110)/6</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N107" s="45">
+      <c r="N110" s="45">
         <v>1</v>
       </c>
-      <c r="Q107" s="43" t="s">
+      <c r="Q110" s="43" t="s">
         <v>753</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
-      <c r="B108" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D108" s="31" t="s">
+    <row r="111" spans="1:17">
+      <c r="B111" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D111" s="31" t="s">
         <v>806</v>
       </c>
-      <c r="E108" s="31" t="s">
+      <c r="E111" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="F108" s="31" t="s">
+      <c r="F111" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="H108" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J108" s="3"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
-      <c r="M108" s="3"/>
-      <c r="N108" s="3"/>
-    </row>
-    <row r="109" spans="1:17">
-      <c r="H109" s="31"/>
-      <c r="I109" s="31"/>
-    </row>
-    <row r="110" spans="1:17">
-      <c r="H110" s="31"/>
-      <c r="I110" s="31"/>
-    </row>
-    <row r="111" spans="1:17">
-      <c r="H111" s="31"/>
-      <c r="I111" s="31"/>
+      <c r="H111" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
     </row>
     <row r="112" spans="1:17">
       <c r="H112" s="31"/>
@@ -10310,8 +10399,20 @@
       <c r="H224" s="31"/>
       <c r="I224" s="31"/>
     </row>
+    <row r="225" spans="8:9">
+      <c r="H225" s="31"/>
+      <c r="I225" s="31"/>
+    </row>
+    <row r="226" spans="8:9">
+      <c r="H226" s="31"/>
+      <c r="I226" s="31"/>
+    </row>
+    <row r="227" spans="8:9">
+      <c r="H227" s="31"/>
+      <c r="I227" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z151"/>
+  <autoFilter ref="A2:Z154"/>
   <mergeCells count="1">
     <mergeCell ref="T1:Y1"/>
   </mergeCells>

</xml_diff>